<commit_message>
modification calcul S1 + cellule diminution SRG
</commit_message>
<xml_diff>
--- a/propre.xlsx
+++ b/propre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\Université\Session-2-H-2020\ACT-1005-Analyse-et-traitement-collectif-du-risque\Calcul-Prestations\ATCR-TP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B466DA90-5377-4DDC-BE0C-E73EEADF5280}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF92E762-DFD5-4C32-99A8-9FF87D770B16}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{47FD59A7-3964-46FC-BE03-C6B259F3D8B0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{47FD59A7-3964-46FC-BE03-C6B259F3D8B0}"/>
   </bookViews>
   <sheets>
     <sheet name="QUESTION 1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="84">
   <si>
     <t>Années</t>
   </si>
@@ -150,9 +150,6 @@
     <t xml:space="preserve">Indexation de la SRG célibataire </t>
   </si>
   <si>
-    <t>Diminution de la SRG selon les autres revenus</t>
-  </si>
-  <si>
     <t>*Les premiers 3500$ du revenu de Virginie ne sont</t>
   </si>
   <si>
@@ -222,25 +219,13 @@
     <t xml:space="preserve">Par contre, il n'aura pas droit à la SRG en raison de ses </t>
   </si>
   <si>
-    <t>revenus trop élevé.</t>
-  </si>
-  <si>
     <t>Calcul de la rente obtenue du RRQ S1</t>
   </si>
   <si>
     <t>Somme des salaires admissibles au S1</t>
   </si>
   <si>
-    <t>Nombres d'années de cotisations au S1</t>
-  </si>
-  <si>
-    <t>Nombres d'années maximum de cotisations au S1</t>
-  </si>
-  <si>
     <t>Rente annuelle S1 de base</t>
-  </si>
-  <si>
-    <t>Facteur d'ajustement acturiel (%)</t>
   </si>
   <si>
     <t>Rente annuelle S1 à 60 ans</t>
@@ -258,9 +243,6 @@
     <t>Calcul de la rente obtenue du RRQ S2</t>
   </si>
   <si>
-    <t xml:space="preserve">Elle n'a pas contribué au S2 pour l'année de 2024, </t>
-  </si>
-  <si>
     <t>Rente de retraite à 60 ans Régime de base</t>
   </si>
   <si>
@@ -276,17 +258,45 @@
     <t>puisque son salaire est demeuré inférieur au MGA.</t>
   </si>
   <si>
-    <t>Pourcentage cible de revenu remplacé (%)</t>
+    <t>Pourcentage cible du revenu remplacé (%)</t>
+  </si>
+  <si>
+    <t>Nombre d'années de cotisations au S1</t>
+  </si>
+  <si>
+    <t>Nombre d'années maximum de cotisations au S1</t>
+  </si>
+  <si>
+    <t>Elle n'a pas contribué au S2 pour l'année de 2024</t>
+  </si>
+  <si>
+    <t>Rente annuelle S1 à 65 ans</t>
+  </si>
+  <si>
+    <t>MGA 2020</t>
+  </si>
+  <si>
+    <t>MGA moyen des 5 dernières années à partir de 2020</t>
+  </si>
+  <si>
+    <t>MGA 2025</t>
+  </si>
+  <si>
+    <t>revenus trop élevés.</t>
+  </si>
+  <si>
+    <t>Montant de la SRG après diminution selon les autres revenus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="#,##0\ &quot;$&quot;"/>
+    <numFmt numFmtId="167" formatCode="_ * #,##0_)\ &quot;$&quot;_ ;_ * \(#,##0\)\ &quot;$&quot;_ ;_ * &quot;-&quot;??_)\ &quot;$&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1025,7 +1035,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1268,12 +1278,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1283,6 +1287,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
@@ -1606,8 +1617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D97A01-C9B7-4676-858F-079C6C4177D4}">
   <dimension ref="B1:R62"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1624,7 +1635,7 @@
     <col min="12" max="13" width="10.88671875" style="1"/>
     <col min="14" max="14" width="48" style="1" customWidth="1"/>
     <col min="15" max="16" width="10.88671875" style="1"/>
-    <col min="17" max="17" width="48.21875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="48.33203125" style="1" customWidth="1"/>
     <col min="18" max="16384" width="10.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -1645,6 +1656,9 @@
       <c r="E2" s="10" t="s">
         <v>3</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="G2" s="36" t="s">
         <v>21</v>
       </c>
@@ -1666,19 +1680,23 @@
         <f>O4</f>
         <v>57400</v>
       </c>
+      <c r="F3" s="125">
+        <f>E3*(1+O6)</f>
+        <v>58978.500000000007</v>
+      </c>
       <c r="G3" s="37">
         <f>D3*($O$9/E3)</f>
-        <v>44991.767880938263</v>
+        <v>46229.041497664068</v>
       </c>
       <c r="L3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="116" t="s">
+      <c r="N3" s="126" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="116"/>
-      <c r="Q3" s="118" t="s">
-        <v>63</v>
+      <c r="O3" s="126"/>
+      <c r="Q3" s="116" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
@@ -1697,7 +1715,7 @@
       </c>
       <c r="G4" s="38">
         <f t="shared" ref="G4:G62" si="0">D4*($O$9/E4)</f>
-        <v>45455.333690171778</v>
+        <v>46705.355366651507</v>
       </c>
       <c r="K4" s="11" t="s">
         <v>13</v>
@@ -1712,9 +1730,9 @@
         <v>57400</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="R4" s="119">
+        <v>74</v>
+      </c>
+      <c r="R4" s="117">
         <v>8.33</v>
       </c>
     </row>
@@ -1734,14 +1752,14 @@
       </c>
       <c r="G5" s="38">
         <f t="shared" si="0"/>
-        <v>46357.549528814736</v>
+        <v>47632.382140857146</v>
       </c>
       <c r="K5" s="12" t="s">
         <v>6</v>
       </c>
       <c r="L5" s="28">
         <f>O16</f>
-        <v>7834.4775121524444</v>
+        <v>7995.0987517423328</v>
       </c>
       <c r="N5" s="12" t="s">
         <v>15</v>
@@ -1750,11 +1768,11 @@
         <v>7217</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="R5" s="120">
-        <f>G3</f>
-        <v>44991.767880938263</v>
+        <v>62</v>
+      </c>
+      <c r="R5" s="118">
+        <f>G3*0.15</f>
+        <v>6934.3562246496103</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
@@ -1773,7 +1791,7 @@
       </c>
       <c r="G6" s="38">
         <f t="shared" si="0"/>
-        <v>46825.745873091299</v>
+        <v>48113.453884601309</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>7</v>
@@ -1788,9 +1806,9 @@
         <v>2.75E-2</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="R6" s="121">
+        <v>75</v>
+      </c>
+      <c r="R6" s="119">
         <v>1</v>
       </c>
     </row>
@@ -1810,7 +1828,7 @@
       </c>
       <c r="G7" s="38">
         <f t="shared" si="0"/>
-        <v>47190.21272850778</v>
+        <v>48487.943578541737</v>
       </c>
       <c r="K7" s="12" t="s">
         <v>8</v>
@@ -1825,9 +1843,9 @@
         <v>10779.84</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="R7" s="121">
+        <v>76</v>
+      </c>
+      <c r="R7" s="119">
         <v>40</v>
       </c>
     </row>
@@ -1847,7 +1865,7 @@
       </c>
       <c r="G8" s="38">
         <f t="shared" si="0"/>
-        <v>47560.873069925779</v>
+        <v>48868.79707934874</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>9</v>
@@ -1863,14 +1881,14 @@
         <v>42</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="R8" s="120">
-        <f>R5*(R4/100)*(R6/R7)</f>
-        <v>93.695356612053942</v>
+        <v>63</v>
+      </c>
+      <c r="R8" s="118">
+        <f>R5*(R4/100)/R7</f>
+        <v>14.440796837832812</v>
       </c>
     </row>
     <row r="9" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -1889,7 +1907,7 @@
       </c>
       <c r="G9" s="38">
         <f t="shared" si="0"/>
-        <v>47628.247380144974</v>
+        <v>48938.024183098962</v>
       </c>
       <c r="K9" s="13" t="s">
         <v>10</v>
@@ -1898,16 +1916,16 @@
         <v>0</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="O9" s="28">
-        <f>AVERAGE(E3:E7)</f>
-        <v>54408.631895356535</v>
+        <f>AVERAGE(E3:E6,F3)</f>
+        <v>55904.869272478842</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="R9" s="121">
+        <v>32</v>
+      </c>
+      <c r="R9" s="119">
         <f>O14</f>
         <v>33</v>
       </c>
@@ -1928,14 +1946,14 @@
       </c>
       <c r="G10" s="38">
         <f t="shared" si="0"/>
-        <v>48471.405812981044</v>
+        <v>49804.369472838029</v>
       </c>
       <c r="K10" s="11" t="s">
         <v>11</v>
       </c>
       <c r="L10" s="70">
         <f>L5</f>
-        <v>7834.4775121524444</v>
+        <v>7995.0987517423328</v>
       </c>
       <c r="N10" s="12" t="s">
         <v>23</v>
@@ -1945,11 +1963,11 @@
         <v>35</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="R10" s="120">
+        <v>64</v>
+      </c>
+      <c r="R10" s="118">
         <f>R8*(1-(R9/100))</f>
-        <v>62.775888930076135</v>
+        <v>9.6753338813479832</v>
       </c>
     </row>
     <row r="11" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -1968,14 +1986,14 @@
       </c>
       <c r="G11" s="38">
         <f t="shared" si="0"/>
-        <v>48962.407838171595</v>
+        <v>50308.874053721316</v>
       </c>
       <c r="K11" s="13" t="s">
         <v>12</v>
       </c>
       <c r="L11" s="17">
         <f>L5/D3</f>
-        <v>0.16505659937875683</v>
+        <v>0.16844056411074873</v>
       </c>
       <c r="N11" s="12" t="s">
         <v>24</v>
@@ -1985,9 +2003,9 @@
         <v>5.25</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="R11" s="119"/>
+        <v>65</v>
+      </c>
+      <c r="R11" s="117"/>
     </row>
     <row r="12" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="62">
@@ -2005,19 +2023,19 @@
       </c>
       <c r="G12" s="38">
         <f t="shared" si="0"/>
-        <v>49383.681003294638</v>
+        <v>50741.732230885231</v>
       </c>
       <c r="N12" s="12" t="s">
         <v>31</v>
       </c>
       <c r="O12" s="69">
         <f>AVERAGE(G3:G24,G32:G39)</f>
-        <v>46398.218646103698</v>
+        <v>47674.169658871557</v>
       </c>
       <c r="Q12" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="R12" s="122"/>
+        <v>66</v>
+      </c>
+      <c r="R12" s="120"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="62">
@@ -2035,7 +2053,7 @@
       </c>
       <c r="G13" s="38">
         <f t="shared" si="0"/>
-        <v>49902.209653829217</v>
+        <v>51274.520419309527</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>33</v>
@@ -2045,7 +2063,7 @@
       </c>
       <c r="O13" s="69">
         <f>O12*0.25</f>
-        <v>11599.554661525925</v>
+        <v>11918.542414717889</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
@@ -2064,10 +2082,10 @@
       </c>
       <c r="G14" s="38">
         <f t="shared" si="0"/>
-        <v>50614.877900308013</v>
+        <v>52006.787042566488</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N14" s="12" t="s">
         <v>32</v>
@@ -2093,17 +2111,17 @@
       </c>
       <c r="G15" s="38">
         <f t="shared" si="0"/>
-        <v>50885.838750420946</v>
+        <v>52285.199316057529</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N15" s="13" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="O15" s="29">
         <f>O13*(1-O14/100)</f>
-        <v>7771.7016232223687</v>
+        <v>7985.423417860985</v>
       </c>
     </row>
     <row r="16" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -2122,14 +2140,14 @@
       </c>
       <c r="G16" s="38">
         <f t="shared" si="0"/>
-        <v>51093.246770174039</v>
-      </c>
-      <c r="N16" s="124" t="s">
-        <v>76</v>
-      </c>
-      <c r="O16" s="125">
+        <v>52498.311056353821</v>
+      </c>
+      <c r="N16" s="122" t="s">
+        <v>70</v>
+      </c>
+      <c r="O16" s="123">
         <f>O15+R10</f>
-        <v>7834.4775121524444</v>
+        <v>7995.0987517423328</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
@@ -2148,7 +2166,7 @@
       </c>
       <c r="G17" s="38">
         <f t="shared" si="0"/>
-        <v>51741.454671530919</v>
+        <v>53164.344674998014</v>
       </c>
       <c r="N17" s="54"/>
       <c r="O17" s="68"/>
@@ -2169,12 +2187,12 @@
       </c>
       <c r="G18" s="38">
         <f t="shared" si="0"/>
-        <v>51835.236058123053</v>
-      </c>
-      <c r="N18" s="116" t="s">
+        <v>53260.705049721444</v>
+      </c>
+      <c r="N18" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="O18" s="116"/>
+      <c r="O18" s="126"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="62">
@@ -2192,7 +2210,7 @@
       </c>
       <c r="G19" s="38">
         <f t="shared" si="0"/>
-        <v>50849.00918549511</v>
+        <v>52247.356938096229</v>
       </c>
       <c r="N19" s="11" t="s">
         <v>18</v>
@@ -2215,7 +2233,7 @@
       </c>
       <c r="G20" s="38">
         <f t="shared" si="0"/>
-        <v>51933.872796467651</v>
+        <v>53362.054298370516</v>
       </c>
       <c r="N20" s="12" t="s">
         <v>19</v>
@@ -2238,7 +2256,7 @@
       </c>
       <c r="G21" s="38">
         <f t="shared" si="0"/>
-        <v>52395.73943180043</v>
+        <v>53836.622266174942</v>
       </c>
       <c r="N21" s="12"/>
       <c r="O21" s="28"/>
@@ -2259,7 +2277,7 @@
       </c>
       <c r="G22" s="38">
         <f t="shared" si="0"/>
-        <v>52008.446568611631</v>
+        <v>53438.678849248448</v>
       </c>
       <c r="N22" s="12" t="s">
         <v>25</v>
@@ -2282,7 +2300,7 @@
       </c>
       <c r="G23" s="38">
         <f t="shared" si="0"/>
-        <v>52758.550209348919</v>
+        <v>54209.41034010602</v>
       </c>
       <c r="N23" s="12" t="s">
         <v>26</v>
@@ -2305,7 +2323,7 @@
       </c>
       <c r="G24" s="38">
         <f t="shared" si="0"/>
-        <v>52204.427545145074</v>
+        <v>53640.049302636573</v>
       </c>
       <c r="N24" s="12"/>
       <c r="O24" s="28"/>
@@ -2349,7 +2367,7 @@
       </c>
       <c r="G26" s="38">
         <f t="shared" si="0"/>
-        <v>2639.4098861728016</v>
+        <v>2711.9936580425538</v>
       </c>
       <c r="N26" s="12"/>
       <c r="O26" s="28"/>
@@ -2370,7 +2388,7 @@
       </c>
       <c r="G27" s="38">
         <f t="shared" si="0"/>
-        <v>2366.6325353695747</v>
+        <v>2431.7149300922379</v>
       </c>
       <c r="N27" s="56" t="s">
         <v>28</v>
@@ -2469,7 +2487,7 @@
       </c>
       <c r="G32" s="38">
         <f t="shared" si="0"/>
-        <v>51741.509821308646</v>
+        <v>53164.40134139463</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
@@ -2488,7 +2506,7 @@
       </c>
       <c r="G33" s="38">
         <f t="shared" si="0"/>
-        <v>53100.680524764924</v>
+        <v>54560.949239195957</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
@@ -2507,7 +2525,7 @@
       </c>
       <c r="G34" s="38">
         <f t="shared" si="0"/>
-        <v>50086.951401581886</v>
+        <v>51464.342565125393</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
@@ -2526,7 +2544,7 @@
       </c>
       <c r="G35" s="38">
         <f t="shared" si="0"/>
-        <v>50230.992307573368</v>
+        <v>51612.344596031639</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
@@ -2545,7 +2563,7 @@
       </c>
       <c r="G36" s="38">
         <f t="shared" si="0"/>
-        <v>48386.573058779664</v>
+        <v>49717.203817896094</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
@@ -2564,7 +2582,7 @@
       </c>
       <c r="G37" s="38">
         <f t="shared" si="0"/>
-        <v>47349.717921805815</v>
+        <v>48651.835164655473</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
@@ -3055,8 +3073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{367AD372-2F5B-444E-901D-D02956C9F1AC}">
   <dimension ref="B1:R62"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView topLeftCell="I12" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3066,7 +3084,7 @@
     <col min="3" max="3" width="11.5546875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.88671875" style="5"/>
     <col min="5" max="5" width="10.88671875" style="6"/>
-    <col min="6" max="6" width="10.88671875" style="1"/>
+    <col min="6" max="6" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.88671875" style="1"/>
     <col min="9" max="9" width="47.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -3074,7 +3092,7 @@
     <col min="11" max="11" width="10.88671875" style="1"/>
     <col min="12" max="12" width="10.88671875" style="1" customWidth="1"/>
     <col min="13" max="13" width="10.88671875" style="1"/>
-    <col min="14" max="14" width="47.88671875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="51.21875" style="1" customWidth="1"/>
     <col min="15" max="16" width="10.88671875" style="1"/>
     <col min="17" max="17" width="43.6640625" style="1" customWidth="1"/>
     <col min="18" max="16384" width="10.88671875" style="1"/>
@@ -3097,6 +3115,9 @@
       <c r="E2" s="10" t="s">
         <v>3</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="G2" s="36" t="s">
         <v>21</v>
       </c>
@@ -3118,19 +3139,23 @@
         <f>O4</f>
         <v>57400</v>
       </c>
+      <c r="F3" s="125">
+        <f>E3*(1+O6)</f>
+        <v>58978.500000000007</v>
+      </c>
       <c r="G3" s="37">
         <f>D3*($O$9/E3)</f>
-        <v>44991.767880938263</v>
+        <v>46229.041497664068</v>
       </c>
       <c r="J3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="116" t="s">
+      <c r="N3" s="126" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="116"/>
-      <c r="Q3" s="118" t="s">
-        <v>63</v>
+      <c r="O3" s="126"/>
+      <c r="Q3" s="116" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
@@ -3149,7 +3174,7 @@
       </c>
       <c r="G4" s="38">
         <f t="shared" ref="G4:G62" si="0">D4*($O$9/E4)</f>
-        <v>45455.333690171778</v>
+        <v>46705.355366651507</v>
       </c>
       <c r="I4" s="11" t="s">
         <v>13</v>
@@ -3164,9 +3189,9 @@
         <v>57400</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="R4" s="119">
+        <v>74</v>
+      </c>
+      <c r="R4" s="117">
         <v>8.33</v>
       </c>
     </row>
@@ -3186,14 +3211,14 @@
       </c>
       <c r="G5" s="38">
         <f t="shared" si="0"/>
-        <v>46357.549528814736</v>
+        <v>47632.382140857146</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>6</v>
       </c>
       <c r="J5" s="28">
         <f>O31</f>
-        <v>8972.6182592112909</v>
+        <v>9156.5734834015293</v>
       </c>
       <c r="N5" s="12" t="s">
         <v>15</v>
@@ -3202,11 +3227,11 @@
         <v>7217</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="R5" s="120">
-        <f>G3</f>
-        <v>44991.767880938263</v>
+        <v>62</v>
+      </c>
+      <c r="R5" s="118">
+        <f>G3*0.15</f>
+        <v>6934.3562246496103</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
@@ -3225,7 +3250,7 @@
       </c>
       <c r="G6" s="38">
         <f t="shared" si="0"/>
-        <v>46825.745873091299</v>
+        <v>48113.453884601309</v>
       </c>
       <c r="I6" s="12" t="s">
         <v>7</v>
@@ -3241,9 +3266,9 @@
         <v>2.75E-2</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="R6" s="121">
+        <v>75</v>
+      </c>
+      <c r="R6" s="119">
         <v>1</v>
       </c>
     </row>
@@ -3263,14 +3288,14 @@
       </c>
       <c r="G7" s="38">
         <f t="shared" si="0"/>
-        <v>47190.21272850778</v>
+        <v>48487.943578541737</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>8</v>
       </c>
       <c r="J7" s="28">
         <f>O34</f>
-        <v>9949.065519136504</v>
+        <v>9857.0879070413866</v>
       </c>
       <c r="N7" s="12" t="s">
         <v>16</v>
@@ -3279,9 +3304,9 @@
         <v>10779.84</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="R7" s="121">
+        <v>76</v>
+      </c>
+      <c r="R7" s="119">
         <v>40</v>
       </c>
     </row>
@@ -3301,7 +3326,7 @@
       </c>
       <c r="G8" s="38">
         <f t="shared" si="0"/>
-        <v>47560.873069925779</v>
+        <v>48868.79707934874</v>
       </c>
       <c r="I8" s="12" t="s">
         <v>9</v>
@@ -3317,14 +3342,14 @@
         <v>42</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="R8" s="120">
-        <f>R5*(R4/100)*(R6/R7)</f>
-        <v>93.695356612053942</v>
+        <v>63</v>
+      </c>
+      <c r="R8" s="118">
+        <f>R5*(R4/100)/R7</f>
+        <v>14.440796837832812</v>
       </c>
     </row>
     <row r="9" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -3343,7 +3368,7 @@
       </c>
       <c r="G9" s="38">
         <f t="shared" si="0"/>
-        <v>47628.247380144974</v>
+        <v>48938.024183098962</v>
       </c>
       <c r="I9" s="13" t="s">
         <v>10</v>
@@ -3355,13 +3380,13 @@
         <v>20</v>
       </c>
       <c r="O9" s="28">
-        <f>AVERAGE(E3:E7)</f>
-        <v>54408.631895356535</v>
+        <f>AVERAGE(E3:E6,F3)</f>
+        <v>55904.869272478842</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="R9" s="121">
+        <v>32</v>
+      </c>
+      <c r="R9" s="119">
         <f>O14</f>
         <v>33</v>
       </c>
@@ -3382,14 +3407,14 @@
       </c>
       <c r="G10" s="38">
         <f t="shared" si="0"/>
-        <v>48471.405812981044</v>
+        <v>49804.369472838029</v>
       </c>
       <c r="I10" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J10" s="70">
         <f>SUM(J5:J7)</f>
-        <v>27414.421039751684</v>
+        <v>27506.398651846805</v>
       </c>
       <c r="N10" s="12" t="s">
         <v>23</v>
@@ -3399,11 +3424,11 @@
         <v>35</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="R10" s="120">
+        <v>64</v>
+      </c>
+      <c r="R10" s="118">
         <f>R8*(1-(R9/100))</f>
-        <v>62.775888930076135</v>
+        <v>9.6753338813479832</v>
       </c>
     </row>
     <row r="11" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -3422,14 +3447,14 @@
       </c>
       <c r="G11" s="38">
         <f t="shared" si="0"/>
-        <v>48962.407838171595</v>
+        <v>50308.874053721316</v>
       </c>
       <c r="I11" s="13" t="s">
         <v>12</v>
       </c>
       <c r="J11" s="17">
         <f>J10/D3</f>
-        <v>0.57756641763793592</v>
+        <v>0.57950419994031033</v>
       </c>
       <c r="N11" s="12" t="s">
         <v>24</v>
@@ -3439,9 +3464,9 @@
         <v>5.25</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="R11" s="119"/>
+        <v>65</v>
+      </c>
+      <c r="R11" s="117"/>
     </row>
     <row r="12" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="62">
@@ -3459,19 +3484,19 @@
       </c>
       <c r="G12" s="38">
         <f t="shared" si="0"/>
-        <v>49383.681003294638</v>
+        <v>50741.732230885231</v>
       </c>
       <c r="N12" s="12" t="s">
         <v>31</v>
       </c>
       <c r="O12" s="69">
         <f>AVERAGE(G3:G24,G32:G39)</f>
-        <v>46398.218646103698</v>
+        <v>47674.169658871557</v>
       </c>
       <c r="Q12" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="R12" s="122"/>
+        <v>66</v>
+      </c>
+      <c r="R12" s="120"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="62">
@@ -3489,14 +3514,14 @@
       </c>
       <c r="G13" s="38">
         <f t="shared" si="0"/>
-        <v>49902.209653829217</v>
+        <v>51274.520419309527</v>
       </c>
       <c r="N13" s="12" t="s">
         <v>30</v>
       </c>
       <c r="O13" s="69">
         <f>O12*0.25</f>
-        <v>11599.554661525925</v>
+        <v>11918.542414717889</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
@@ -3515,7 +3540,7 @@
       </c>
       <c r="G14" s="38">
         <f t="shared" si="0"/>
-        <v>50614.877900308013</v>
+        <v>52006.787042566488</v>
       </c>
       <c r="N14" s="12" t="s">
         <v>32</v>
@@ -3541,14 +3566,14 @@
       </c>
       <c r="G15" s="38">
         <f t="shared" si="0"/>
-        <v>50885.838750420946</v>
+        <v>52285.199316057529</v>
       </c>
       <c r="N15" s="13" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="O15" s="29">
         <f>O13*(1-O14/100)</f>
-        <v>7771.7016232223687</v>
+        <v>7985.423417860985</v>
       </c>
     </row>
     <row r="16" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -3567,14 +3592,14 @@
       </c>
       <c r="G16" s="38">
         <f t="shared" si="0"/>
-        <v>51093.246770174039</v>
-      </c>
-      <c r="N16" s="126" t="s">
-        <v>76</v>
-      </c>
-      <c r="O16" s="125">
+        <v>52498.311056353821</v>
+      </c>
+      <c r="N16" s="124" t="s">
+        <v>70</v>
+      </c>
+      <c r="O16" s="123">
         <f>O15+R10</f>
-        <v>7834.4775121524444</v>
+        <v>7995.0987517423328</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
@@ -3593,7 +3618,7 @@
       </c>
       <c r="G17" s="38">
         <f t="shared" si="0"/>
-        <v>51741.454671530919</v>
+        <v>53164.344674998014</v>
       </c>
       <c r="N17" s="54"/>
       <c r="O17" s="68"/>
@@ -3614,12 +3639,12 @@
       </c>
       <c r="G18" s="38">
         <f t="shared" si="0"/>
-        <v>51835.236058123053</v>
-      </c>
-      <c r="N18" s="116" t="s">
+        <v>53260.705049721444</v>
+      </c>
+      <c r="N18" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="O18" s="116"/>
+      <c r="O18" s="126"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="62">
@@ -3637,7 +3662,7 @@
       </c>
       <c r="G19" s="38">
         <f t="shared" si="0"/>
-        <v>50849.00918549511</v>
+        <v>52247.356938096229</v>
       </c>
       <c r="N19" s="11" t="s">
         <v>18</v>
@@ -3660,7 +3685,7 @@
       </c>
       <c r="G20" s="38">
         <f t="shared" si="0"/>
-        <v>51933.872796467651</v>
+        <v>53362.054298370516</v>
       </c>
       <c r="N20" s="12" t="s">
         <v>19</v>
@@ -3683,7 +3708,7 @@
       </c>
       <c r="G21" s="38">
         <f t="shared" si="0"/>
-        <v>52395.73943180043</v>
+        <v>53836.622266174942</v>
       </c>
       <c r="N21" s="12"/>
       <c r="O21" s="28"/>
@@ -3704,7 +3729,7 @@
       </c>
       <c r="G22" s="38">
         <f t="shared" si="0"/>
-        <v>52008.446568611631</v>
+        <v>53438.678849248448</v>
       </c>
       <c r="N22" s="12" t="s">
         <v>25</v>
@@ -3727,7 +3752,7 @@
       </c>
       <c r="G23" s="38">
         <f t="shared" si="0"/>
-        <v>52758.550209348919</v>
+        <v>54209.41034010602</v>
       </c>
       <c r="N23" s="12" t="s">
         <v>26</v>
@@ -3750,7 +3775,7 @@
       </c>
       <c r="G24" s="38">
         <f t="shared" si="0"/>
-        <v>52204.427545145074</v>
+        <v>53640.049302636573</v>
       </c>
       <c r="N24" s="12"/>
       <c r="O24" s="28"/>
@@ -3794,7 +3819,7 @@
       </c>
       <c r="G26" s="38">
         <f t="shared" si="0"/>
-        <v>2639.4098861728016</v>
+        <v>2711.9936580425538</v>
       </c>
       <c r="N26" s="12"/>
       <c r="O26" s="28"/>
@@ -3815,7 +3840,7 @@
       </c>
       <c r="G27" s="38">
         <f t="shared" si="0"/>
-        <v>2366.6325353695747</v>
+        <v>2431.7149300922379</v>
       </c>
       <c r="N27" s="56" t="s">
         <v>28</v>
@@ -3880,10 +3905,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N30" s="116" t="s">
-        <v>44</v>
-      </c>
-      <c r="O30" s="117"/>
+      <c r="N30" s="126" t="s">
+        <v>43</v>
+      </c>
+      <c r="O30" s="127"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="22">
@@ -3908,7 +3933,7 @@
       </c>
       <c r="O31" s="75">
         <f>O16*(1+O6)^5</f>
-        <v>8972.6182592112909</v>
+        <v>9156.5734834015293</v>
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
@@ -3927,7 +3952,7 @@
       </c>
       <c r="G32" s="38">
         <f t="shared" si="0"/>
-        <v>51741.509821308646</v>
+        <v>53164.40134139463</v>
       </c>
       <c r="N32" s="78" t="s">
         <v>36</v>
@@ -3953,7 +3978,7 @@
       </c>
       <c r="G33" s="38">
         <f t="shared" si="0"/>
-        <v>53100.680524764924</v>
+        <v>54560.949239195957</v>
       </c>
       <c r="N33" s="78" t="s">
         <v>37</v>
@@ -3979,14 +4004,14 @@
       </c>
       <c r="G34" s="38">
         <f t="shared" si="0"/>
-        <v>50086.951401581886</v>
+        <v>51464.342565125393</v>
       </c>
       <c r="N34" s="79" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="O34" s="80">
         <f>O33-((O31-3500)/2)</f>
-        <v>9949.065519136504</v>
+        <v>9857.0879070413866</v>
       </c>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
@@ -4005,10 +4030,10 @@
       </c>
       <c r="G35" s="38">
         <f t="shared" si="0"/>
-        <v>50230.992307573368</v>
+        <v>51612.344596031639</v>
       </c>
       <c r="N35" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O35" s="55"/>
     </row>
@@ -4028,10 +4053,10 @@
       </c>
       <c r="G36" s="38">
         <f t="shared" si="0"/>
-        <v>48386.573058779664</v>
+        <v>49717.203817896094</v>
       </c>
       <c r="N36" s="54" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O36" s="73"/>
     </row>
@@ -4051,7 +4076,7 @@
       </c>
       <c r="G37" s="38">
         <f t="shared" si="0"/>
-        <v>47349.717921805815</v>
+        <v>48651.835164655473</v>
       </c>
       <c r="N37" s="54"/>
       <c r="O37" s="72"/>
@@ -4553,8 +4578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF3058D-9527-44EF-BE25-5C09CA35E4DB}">
   <dimension ref="B1:R67"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4564,13 +4589,13 @@
     <col min="3" max="3" width="11.5546875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="5" customWidth="1"/>
     <col min="5" max="5" width="11" style="6" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" style="1"/>
+    <col min="6" max="6" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.88671875" style="1"/>
     <col min="9" max="9" width="47.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="10.88671875" style="1"/>
-    <col min="13" max="13" width="48" style="1" customWidth="1"/>
+    <col min="13" max="13" width="49.5546875" style="1" customWidth="1"/>
     <col min="14" max="16" width="10.88671875" style="1"/>
     <col min="17" max="17" width="43.88671875" style="1" customWidth="1"/>
     <col min="18" max="16384" width="10.88671875" style="1"/>
@@ -4593,6 +4618,9 @@
       <c r="E2" s="10" t="s">
         <v>3</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="G2" s="89" t="s">
         <v>21</v>
       </c>
@@ -4615,19 +4643,23 @@
         <f t="shared" ref="E3:E6" si="1">E4*(1+$N$6)</f>
         <v>65738.689948352316</v>
       </c>
+      <c r="F3" s="125">
+        <f>E3*(1+N6)</f>
+        <v>67546.503921932002</v>
+      </c>
       <c r="G3" s="90">
         <f>D3*($N$9/E3)</f>
-        <v>51527.872455631288</v>
+        <v>52944.888948161155</v>
       </c>
       <c r="J3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="116" t="s">
+      <c r="M3" s="126" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="116"/>
-      <c r="Q3" s="118" t="s">
-        <v>72</v>
+      <c r="N3" s="126"/>
+      <c r="Q3" s="116" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
@@ -4647,7 +4679,7 @@
       </c>
       <c r="G4" s="90">
         <f t="shared" ref="G4:G66" si="2">D4*($N$9/E4)</f>
-        <v>51527.872455631288</v>
+        <v>52944.888948161155</v>
       </c>
       <c r="I4" s="11" t="s">
         <v>13</v>
@@ -4662,9 +4694,9 @@
         <v>57400</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="R4" s="119">
+        <v>74</v>
+      </c>
+      <c r="R4" s="117">
         <v>8.33</v>
       </c>
     </row>
@@ -4685,14 +4717,14 @@
       </c>
       <c r="G5" s="90">
         <f t="shared" si="2"/>
-        <v>51527.872455631295</v>
+        <v>52944.888948161162</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>6</v>
       </c>
       <c r="J5" s="28">
         <f>N16</f>
-        <v>17479.211164755223</v>
+        <v>14398.564752910162</v>
       </c>
       <c r="M5" s="12" t="s">
         <v>15</v>
@@ -4701,11 +4733,11 @@
         <v>7217</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="R5" s="120">
-        <f>SUM(G3:G8)</f>
-        <v>309167.23473378771</v>
+        <v>62</v>
+      </c>
+      <c r="R5" s="118">
+        <f>G8*0.15+G7*0.3+G6*0.5+G5*0.75+G4+G3</f>
+        <v>195896.08910819629</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
@@ -4725,7 +4757,7 @@
       </c>
       <c r="G6" s="90">
         <f t="shared" si="2"/>
-        <v>51527.872455631295</v>
+        <v>52944.888948161162</v>
       </c>
       <c r="I6" s="12" t="s">
         <v>7</v>
@@ -4741,9 +4773,9 @@
         <v>2.75E-2</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="R6" s="121">
+        <v>75</v>
+      </c>
+      <c r="R6" s="119">
         <f>B3-B8+1</f>
         <v>6</v>
       </c>
@@ -4765,14 +4797,14 @@
       </c>
       <c r="G7" s="90">
         <f t="shared" si="2"/>
-        <v>51527.872455631295</v>
+        <v>52944.888948161155</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>8</v>
       </c>
       <c r="J7" s="28">
         <f>N33</f>
-        <v>5695.769066364539</v>
+        <v>7236.0922722870691</v>
       </c>
       <c r="M7" s="12" t="s">
         <v>16</v>
@@ -4781,9 +4813,9 @@
         <v>10779.84</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="R7" s="121">
+        <v>76</v>
+      </c>
+      <c r="R7" s="119">
         <v>40</v>
       </c>
     </row>
@@ -4802,7 +4834,7 @@
       </c>
       <c r="G8" s="90">
         <f t="shared" si="2"/>
-        <v>51527.872455631288</v>
+        <v>52944.888948161148</v>
       </c>
       <c r="I8" s="12" t="s">
         <v>9</v>
@@ -4811,21 +4843,21 @@
         <v>0</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N8" s="31">
         <f>65-18</f>
         <v>47</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="R8" s="120">
-        <f>R5*(R4/100)*(R6/R7)</f>
-        <v>3863.0445979986771</v>
+        <v>63</v>
+      </c>
+      <c r="R8" s="118">
+        <f>R5*(R4/100)/R7</f>
+        <v>407.95360556781873</v>
       </c>
     </row>
     <row r="9" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -4844,7 +4876,7 @@
       </c>
       <c r="G9" s="90">
         <f t="shared" si="2"/>
-        <v>52058.782020158455</v>
+        <v>53490.398525712815</v>
       </c>
       <c r="I9" s="13" t="s">
         <v>10</v>
@@ -4856,13 +4888,13 @@
         <v>20</v>
       </c>
       <c r="N9" s="28">
-        <f>AVERAGE(E3:E7)</f>
-        <v>62312.755795868907</v>
+        <f>AVERAGE(E3:E6,F3)</f>
+        <v>64026.356580255306</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="R9" s="121">
+        <v>32</v>
+      </c>
+      <c r="R9" s="119">
         <f>N14</f>
         <v>0</v>
       </c>
@@ -4883,14 +4915,14 @@
       </c>
       <c r="G10" s="90">
         <f t="shared" si="2"/>
-        <v>53092.065770734102</v>
+        <v>54552.09757942929</v>
       </c>
       <c r="I10" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J10" s="70">
         <f>SUM(J5:J7)</f>
-        <v>31667.717492523654</v>
+        <v>30127.39428660112</v>
       </c>
       <c r="M10" s="12" t="s">
         <v>23</v>
@@ -4900,11 +4932,11 @@
         <v>40</v>
       </c>
       <c r="Q10" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="R10" s="123">
+        <v>78</v>
+      </c>
+      <c r="R10" s="121">
         <f>R8*(1-(R9/100))</f>
-        <v>3863.0445979986771</v>
+        <v>407.95360556781873</v>
       </c>
     </row>
     <row r="11" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -4923,14 +4955,14 @@
       </c>
       <c r="G11" s="90">
         <f t="shared" si="2"/>
-        <v>53628.278563614738</v>
+        <v>55103.056224114152</v>
       </c>
       <c r="I11" s="13" t="s">
         <v>12</v>
       </c>
       <c r="J11" s="17">
         <f>J10/D3</f>
-        <v>0.58254632130784378</v>
+        <v>0.5542111684049823</v>
       </c>
       <c r="M11" s="12" t="s">
         <v>24</v>
@@ -4956,16 +4988,16 @@
       </c>
       <c r="G12" s="90">
         <f t="shared" si="2"/>
-        <v>54045.692737912206</v>
+        <v>55531.9492882048</v>
       </c>
       <c r="M12" s="12" t="s">
         <v>31</v>
       </c>
       <c r="N12" s="69">
         <f>AVERAGE(G3:G29,G37:G43)</f>
-        <v>54464.666267026179</v>
-      </c>
-      <c r="Q12" s="118"/>
+        <v>55962.444589369377</v>
+      </c>
+      <c r="Q12" s="116"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="62">
@@ -4983,17 +5015,17 @@
       </c>
       <c r="G13" s="90">
         <f t="shared" si="2"/>
-        <v>54470.200146633957</v>
+        <v>55968.130650666404</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M13" s="12" t="s">
         <v>30</v>
       </c>
       <c r="N13" s="69">
         <f>N12*0.25</f>
-        <v>13616.166566756545</v>
+        <v>13990.611147342344</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
@@ -5012,7 +5044,7 @@
       </c>
       <c r="G14" s="90">
         <f t="shared" si="2"/>
-        <v>54547.362148201624</v>
+        <v>56047.414607277169</v>
       </c>
       <c r="M14" s="12" t="s">
         <v>32</v>
@@ -5037,17 +5069,17 @@
       </c>
       <c r="G15" s="90">
         <f t="shared" si="2"/>
-        <v>55513.009026138025</v>
+        <v>57039.616774356829</v>
       </c>
       <c r="M15" s="13" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="N15" s="29">
         <f>N13*(1-N14/100)</f>
-        <v>13616.166566756545</v>
-      </c>
-      <c r="Q15" s="118" t="s">
-        <v>73</v>
+        <v>13990.611147342344</v>
+      </c>
+      <c r="Q15" s="116" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -5066,17 +5098,17 @@
       </c>
       <c r="G16" s="90">
         <f t="shared" si="2"/>
-        <v>56075.340557462318</v>
-      </c>
-      <c r="M16" s="124" t="s">
-        <v>78</v>
-      </c>
-      <c r="N16" s="125">
+        <v>57617.412422792535</v>
+      </c>
+      <c r="M16" s="122" t="s">
+        <v>72</v>
+      </c>
+      <c r="N16" s="123">
         <f>N15+R10</f>
-        <v>17479.211164755223</v>
+        <v>14398.564752910162</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
@@ -5095,12 +5127,12 @@
       </c>
       <c r="G17" s="90">
         <f t="shared" si="2"/>
-        <v>56557.813484040445</v>
+        <v>58113.153354851558</v>
       </c>
       <c r="M17" s="54"/>
       <c r="N17" s="68"/>
       <c r="Q17" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="2:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -5119,12 +5151,12 @@
       </c>
       <c r="G18" s="90">
         <f t="shared" si="2"/>
-        <v>57151.670525622867</v>
-      </c>
-      <c r="M18" s="116" t="s">
+        <v>58723.341465077501</v>
+      </c>
+      <c r="M18" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="N18" s="116"/>
+      <c r="N18" s="126"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="62">
@@ -5142,7 +5174,7 @@
       </c>
       <c r="G19" s="90">
         <f t="shared" si="2"/>
-        <v>57967.870471464419</v>
+        <v>59561.986909429696</v>
       </c>
       <c r="M19" s="11" t="s">
         <v>18</v>
@@ -5165,7 +5197,7 @@
       </c>
       <c r="G20" s="90">
         <f t="shared" si="2"/>
-        <v>58278.194710379335</v>
+        <v>59880.845064914771</v>
       </c>
       <c r="M20" s="12" t="s">
         <v>19</v>
@@ -5188,7 +5220,7 @@
       </c>
       <c r="G21" s="90">
         <f t="shared" si="2"/>
-        <v>58515.733586744311</v>
+        <v>60124.916260379796</v>
       </c>
       <c r="M21" s="12"/>
       <c r="N21" s="28"/>
@@ -5209,7 +5241,7 @@
       </c>
       <c r="G22" s="90">
         <f t="shared" si="2"/>
-        <v>59258.108817569606</v>
+        <v>60887.706810052783</v>
       </c>
       <c r="M22" s="12" t="s">
         <v>25</v>
@@ -5232,7 +5264,7 @@
       </c>
       <c r="G23" s="90">
         <f t="shared" si="2"/>
-        <v>59365.514139801453</v>
+        <v>60998.065778645992</v>
       </c>
       <c r="M23" s="12" t="s">
         <v>26</v>
@@ -5255,7 +5287,7 @@
       </c>
       <c r="G24" s="90">
         <f t="shared" si="2"/>
-        <v>58236.01479139689</v>
+        <v>59837.505198160303</v>
       </c>
       <c r="M24" s="12"/>
       <c r="N24" s="28"/>
@@ -5276,7 +5308,7 @@
       </c>
       <c r="G25" s="90">
         <f t="shared" si="2"/>
-        <v>59478.480166971349</v>
+        <v>61114.138371563065</v>
       </c>
       <c r="M25" s="12" t="s">
         <v>27</v>
@@ -5299,7 +5331,7 @@
       </c>
       <c r="G26" s="90">
         <f t="shared" si="2"/>
-        <v>60007.443712923086</v>
+        <v>61657.648415028474</v>
       </c>
       <c r="M26" s="12"/>
       <c r="N26" s="28"/>
@@ -5320,7 +5352,7 @@
       </c>
       <c r="G27" s="90">
         <f t="shared" si="2"/>
-        <v>59563.88752037294</v>
+        <v>61201.894427183201</v>
       </c>
       <c r="M27" s="56" t="s">
         <v>28</v>
@@ -5343,7 +5375,7 @@
       </c>
       <c r="G28" s="90">
         <f t="shared" si="2"/>
-        <v>60422.961225382693</v>
+        <v>62084.592659080721</v>
       </c>
       <c r="M28" s="54"/>
       <c r="N28" s="55"/>
@@ -5364,7 +5396,7 @@
       </c>
       <c r="G29" s="90">
         <f t="shared" si="2"/>
-        <v>59788.339308737188</v>
+        <v>61432.518639727467</v>
       </c>
     </row>
     <row r="30" spans="2:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -5385,10 +5417,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M30" s="116" t="s">
-        <v>44</v>
-      </c>
-      <c r="N30" s="117"/>
+      <c r="M30" s="126" t="s">
+        <v>43</v>
+      </c>
+      <c r="N30" s="127"/>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B31" s="22">
@@ -5406,7 +5438,7 @@
       </c>
       <c r="G31" s="90">
         <f t="shared" si="2"/>
-        <v>3022.8457866503422</v>
+        <v>3105.9740457832272</v>
       </c>
       <c r="M31" s="77" t="s">
         <v>36</v>
@@ -5432,7 +5464,7 @@
       </c>
       <c r="G32" s="90">
         <f t="shared" si="2"/>
-        <v>2710.4411579153898</v>
+        <v>2784.9782897580635</v>
       </c>
       <c r="M32" s="78" t="s">
         <v>37</v>
@@ -5461,11 +5493,11 @@
         <v>0</v>
       </c>
       <c r="M33" s="79" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="N33" s="80">
         <f>N32-((N16-3500)/2)</f>
-        <v>5695.769066364539</v>
+        <v>7236.0922722870691</v>
       </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
@@ -5487,7 +5519,7 @@
         <v>0</v>
       </c>
       <c r="M34" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N34" s="55"/>
     </row>
@@ -5510,7 +5542,7 @@
         <v>0</v>
       </c>
       <c r="M35" s="54" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N35" s="73"/>
     </row>
@@ -5549,7 +5581,7 @@
       </c>
       <c r="G37" s="90">
         <f t="shared" si="2"/>
-        <v>59258.171979139981</v>
+        <v>60887.771708566332</v>
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
@@ -5568,7 +5600,7 @@
       </c>
       <c r="G38" s="90">
         <f t="shared" si="2"/>
-        <v>60814.793955819347</v>
+        <v>62487.200789604387</v>
       </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
@@ -5587,7 +5619,7 @@
       </c>
       <c r="G39" s="90">
         <f t="shared" si="2"/>
-        <v>57363.250324856825</v>
+        <v>58940.739708790381</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
@@ -5606,7 +5638,7 @@
       </c>
       <c r="G40" s="90">
         <f t="shared" si="2"/>
-        <v>57528.216534941384</v>
+        <v>59110.242489652272</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
@@ -5625,7 +5657,7 @@
       </c>
       <c r="G41" s="90">
         <f t="shared" si="2"/>
-        <v>55415.852334049006</v>
+        <v>56939.788273235361</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
@@ -5644,7 +5676,7 @@
       </c>
       <c r="G42" s="90">
         <f t="shared" si="2"/>
-        <v>54228.369784033675</v>
+        <v>55719.649953094602</v>
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
@@ -6132,8 +6164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D06BBD0-3540-47FD-9C64-4AC625E42B0E}">
   <dimension ref="B1:T62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="72" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -6145,7 +6177,7 @@
     <col min="5" max="5" width="10.88671875" style="6"/>
     <col min="6" max="6" width="12.5546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" style="1"/>
+    <col min="8" max="8" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="47.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="10.88671875" style="1"/>
@@ -6171,11 +6203,14 @@
         <v>3</v>
       </c>
       <c r="F2" s="89" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G2" s="110" t="s">
         <v>21</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="I2" s="1" t="s">
         <v>4</v>
       </c>
@@ -6183,7 +6218,7 @@
         <v>0</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>2</v>
@@ -6192,7 +6227,7 @@
         <v>3</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="2:20" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6211,15 +6246,19 @@
       <c r="F3" s="86"/>
       <c r="G3" s="111">
         <f>D3*($N$9/E3)</f>
-        <v>46219.848429433448</v>
+        <v>47490.894261242873</v>
+      </c>
+      <c r="H3" s="125">
+        <f>E3*(1+N6)</f>
+        <v>58978.500000000007</v>
       </c>
       <c r="J3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="116" t="s">
+      <c r="M3" s="126" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="116"/>
+      <c r="N3" s="126"/>
       <c r="P3" s="2">
         <v>2019</v>
       </c>
@@ -6250,7 +6289,7 @@
       <c r="F4" s="87"/>
       <c r="G4" s="111">
         <f t="shared" ref="G4:G22" si="0">D4*($N$9/E4)</f>
-        <v>46696.149081341428</v>
+        <v>47980.293181078327</v>
       </c>
       <c r="I4" s="11" t="s">
         <v>13</v>
@@ -6296,14 +6335,14 @@
       <c r="F5" s="87"/>
       <c r="G5" s="111">
         <f t="shared" si="0"/>
-        <v>47623.030386925755</v>
+        <v>48932.663722566213</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>6</v>
       </c>
       <c r="J5" s="28">
         <f>N16</f>
-        <v>8390.5652658961444</v>
+        <v>8532.345452032805</v>
       </c>
       <c r="M5" s="12" t="s">
         <v>15</v>
@@ -6342,7 +6381,7 @@
       <c r="F6" s="87"/>
       <c r="G6" s="111">
         <f t="shared" si="0"/>
-        <v>48103.88909534111</v>
+        <v>49426.746045462991</v>
       </c>
       <c r="I6" s="12" t="s">
         <v>7</v>
@@ -6387,7 +6426,7 @@
       <c r="F7" s="87"/>
       <c r="G7" s="111">
         <f t="shared" si="0"/>
-        <v>48477.979042153478</v>
+        <v>49811.123465812692</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>8</v>
@@ -6432,7 +6471,7 @@
       <c r="F8" s="87"/>
       <c r="G8" s="111">
         <f t="shared" si="0"/>
-        <v>48859.062719593581</v>
+        <v>50202.686944382411</v>
       </c>
       <c r="I8" s="12" t="s">
         <v>9</v>
@@ -6448,7 +6487,7 @@
         <v>42</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P8" s="2">
         <v>2014</v>
@@ -6481,7 +6520,7 @@
       <c r="F9" s="87"/>
       <c r="G9" s="111">
         <f t="shared" si="0"/>
-        <v>48927.737021538662</v>
+        <v>50273.249789630972</v>
       </c>
       <c r="I9" s="13" t="s">
         <v>10</v>
@@ -6493,8 +6532,8 @@
         <v>20</v>
       </c>
       <c r="N9" s="28">
-        <f>AVERAGE(E3:E7)</f>
-        <v>54408.631895356535</v>
+        <f>AVERAGE(E3:E6,H3)</f>
+        <v>55904.869272478842</v>
       </c>
       <c r="P9" s="2">
         <v>2013</v>
@@ -6527,14 +6566,14 @@
       <c r="F10" s="87"/>
       <c r="G10" s="111">
         <f t="shared" si="0"/>
-        <v>49794.173134240089</v>
+        <v>51163.512895431697</v>
       </c>
       <c r="I10" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J10" s="70">
         <f>SUM(J4:J5)</f>
-        <v>35261.829265896144</v>
+        <v>35403.609452032804</v>
       </c>
       <c r="M10" s="12" t="s">
         <v>23</v>
@@ -6574,14 +6613,14 @@
       <c r="F11" s="87"/>
       <c r="G11" s="111">
         <f t="shared" si="0"/>
-        <v>50299.129097953301</v>
+        <v>51682.355148147013</v>
       </c>
       <c r="I11" s="13" t="s">
         <v>12</v>
       </c>
       <c r="J11" s="17">
         <f>J10/D3</f>
-        <v>0.72315640093304367</v>
+        <v>0.72606405635718718</v>
       </c>
       <c r="M11" s="12" t="s">
         <v>24</v>
@@ -6621,14 +6660,14 @@
       <c r="F12" s="87"/>
       <c r="G12" s="111">
         <f t="shared" si="0"/>
-        <v>50731.279779481454</v>
+        <v>52126.389973417186</v>
       </c>
       <c r="M12" s="12" t="s">
         <v>31</v>
       </c>
       <c r="N12" s="69">
         <f>AVERAGE(G3:G38)</f>
-        <v>49518.283173384189</v>
+        <v>50880.035960652254</v>
       </c>
       <c r="P12" s="2">
         <v>2010</v>
@@ -6661,17 +6700,17 @@
       <c r="F13" s="87"/>
       <c r="G13" s="111">
         <f t="shared" si="0"/>
-        <v>51263.543180459317</v>
+        <v>52673.29061792195</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M13" s="12" t="s">
         <v>30</v>
       </c>
       <c r="N13" s="69">
         <f>N12*0.25</f>
-        <v>12379.570793346047</v>
+        <v>12720.008990163064</v>
       </c>
       <c r="P13" s="2">
         <v>2009</v>
@@ -6704,10 +6743,10 @@
       <c r="F14" s="87"/>
       <c r="G14" s="111">
         <f t="shared" si="0"/>
-        <v>51996.223193894533</v>
+        <v>53426.11933172663</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M14" s="12" t="s">
         <v>32</v>
@@ -6747,14 +6786,14 @@
       <c r="F15" s="87"/>
       <c r="G15" s="111">
         <f t="shared" si="0"/>
-        <v>52274.954606309591</v>
+        <v>53712.515857983111</v>
       </c>
       <c r="M15" s="13" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="N15" s="29">
         <f>N13*(1-N14/100)</f>
-        <v>8294.3124315418499</v>
+        <v>8522.4060234092522</v>
       </c>
       <c r="P15" s="2">
         <v>2007</v>
@@ -6787,17 +6826,17 @@
       <c r="F16" s="87"/>
       <c r="G16" s="111">
         <f t="shared" si="0"/>
-        <v>52487.883983556276</v>
+        <v>53931.30079310407</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="M16" s="124" t="s">
-        <v>76</v>
-      </c>
-      <c r="N16" s="125">
+        <v>60</v>
+      </c>
+      <c r="M16" s="122" t="s">
+        <v>70</v>
+      </c>
+      <c r="N16" s="123">
         <f>N15+N45</f>
-        <v>8390.5652658961444</v>
+        <v>8532.345452032805</v>
       </c>
       <c r="P16" s="2">
         <v>2006</v>
@@ -6830,10 +6869,10 @@
       <c r="F17" s="87"/>
       <c r="G17" s="111">
         <f t="shared" si="0"/>
-        <v>53153.865231654549</v>
+        <v>54615.596525525048</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="J17" s="115"/>
       <c r="M17" s="54"/>
@@ -6869,12 +6908,12 @@
       <c r="F18" s="87"/>
       <c r="G18" s="111">
         <f t="shared" si="0"/>
-        <v>53250.064221114306</v>
-      </c>
-      <c r="M18" s="116" t="s">
+        <v>54714.440987194954</v>
+      </c>
+      <c r="M18" s="126" t="s">
         <v>17</v>
       </c>
-      <c r="N18" s="116"/>
+      <c r="N18" s="126"/>
       <c r="P18" s="2">
         <v>2004</v>
       </c>
@@ -6906,10 +6945,10 @@
       <c r="F19" s="87"/>
       <c r="G19" s="111">
         <f t="shared" si="0"/>
-        <v>52237.462925015607</v>
+        <v>53673.993155453536</v>
       </c>
       <c r="M19" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N19" s="32"/>
       <c r="P19" s="2">
@@ -6943,11 +6982,11 @@
       <c r="F20" s="87"/>
       <c r="G20" s="111">
         <f t="shared" si="0"/>
-        <v>53350.78263202696</v>
+        <v>54817.929154407706</v>
       </c>
       <c r="J20" s="35"/>
       <c r="M20" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N20" s="33"/>
       <c r="P20" s="2">
@@ -6981,7 +7020,7 @@
       <c r="F21" s="87"/>
       <c r="G21" s="111">
         <f t="shared" si="0"/>
-        <v>53826.266652868369</v>
+        <v>55306.488985822252</v>
       </c>
       <c r="M21" s="12"/>
       <c r="N21" s="28"/>
@@ -7016,7 +7055,7 @@
       <c r="F22" s="87"/>
       <c r="G22" s="111">
         <f t="shared" si="0"/>
-        <v>53427.334884774427</v>
+        <v>54896.586594105727</v>
       </c>
       <c r="M22" s="12" t="s">
         <v>25</v>
@@ -7056,7 +7095,7 @@
       </c>
       <c r="G23" s="111">
         <f>F23*($N$9/E23)</f>
-        <v>54469.325040243748</v>
+        <v>55967.231478850452</v>
       </c>
       <c r="M23" s="12" t="s">
         <v>26</v>
@@ -7095,8 +7134,8 @@
         <v>32166</v>
       </c>
       <c r="G24" s="111">
-        <f t="shared" ref="G24:G37" si="4">F24*($N$9/E24)</f>
-        <v>53897.846404260468</v>
+        <f>F24*($N$9/E24)</f>
+        <v>55380.037180377636</v>
       </c>
       <c r="M24" s="12"/>
       <c r="N24" s="28"/>
@@ -7133,8 +7172,8 @@
         <v>31473.5</v>
       </c>
       <c r="G25" s="111">
-        <f t="shared" si="4"/>
-        <v>54187.763483075782</v>
+        <f t="shared" ref="G25:G37" si="4">F25*($N$9/E25)</f>
+        <v>55677.926978860363</v>
       </c>
       <c r="M25" s="12" t="s">
         <v>27</v>
@@ -7174,7 +7213,7 @@
       </c>
       <c r="G26" s="111">
         <f t="shared" si="4"/>
-        <v>54408.639717916012</v>
+        <v>55904.877310158699</v>
       </c>
       <c r="M26" s="12"/>
       <c r="N26" s="28"/>
@@ -7212,7 +7251,7 @@
       </c>
       <c r="G27" s="111">
         <f t="shared" si="4"/>
-        <v>53110.178751686573</v>
+        <v>54570.708667357954</v>
       </c>
       <c r="M27" s="56" t="s">
         <v>28</v>
@@ -7252,7 +7291,7 @@
       </c>
       <c r="G28" s="111">
         <f t="shared" si="4"/>
-        <v>53038.28001901642</v>
+        <v>54496.832719539365</v>
       </c>
       <c r="P28" s="22">
         <v>1994</v>
@@ -7288,10 +7327,10 @@
       </c>
       <c r="G29" s="111">
         <f t="shared" si="4"/>
-        <v>53119.923166885324</v>
-      </c>
-      <c r="M29" s="116"/>
-      <c r="N29" s="117"/>
+        <v>54580.721053974674</v>
+      </c>
+      <c r="M29" s="126"/>
+      <c r="N29" s="127"/>
       <c r="P29" s="22">
         <v>1993</v>
       </c>
@@ -7326,12 +7365,12 @@
       </c>
       <c r="G30" s="111">
         <f t="shared" si="4"/>
-        <v>53226.086731470365</v>
-      </c>
-      <c r="M30" s="116" t="s">
-        <v>46</v>
-      </c>
-      <c r="N30" s="117"/>
+        <v>54689.804116585801</v>
+      </c>
+      <c r="M30" s="126" t="s">
+        <v>45</v>
+      </c>
+      <c r="N30" s="127"/>
       <c r="P30" s="22">
         <v>1992</v>
       </c>
@@ -7366,10 +7405,10 @@
       </c>
       <c r="G31" s="111">
         <f t="shared" si="4"/>
-        <v>53797.335236545936</v>
+        <v>55276.761955550952</v>
       </c>
       <c r="M31" s="77" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N31" s="75">
         <f>AVERAGE(D3:D7)</f>
@@ -7409,10 +7448,10 @@
       </c>
       <c r="G32" s="111">
         <f t="shared" si="4"/>
-        <v>53418.798258592833</v>
+        <v>54887.815210704131</v>
       </c>
       <c r="M32" s="78" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N32" s="92">
         <f>60-18</f>
@@ -7452,17 +7491,17 @@
       </c>
       <c r="G33" s="111">
         <f>H33*($N$9/E33)</f>
-        <v>54408.631895356535</v>
+        <v>55904.869272478842</v>
       </c>
       <c r="H33" s="35">
         <f>E33</f>
         <v>25436.47790299587</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M33" s="78" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N33" s="93">
         <v>1.35E-2</v>
@@ -7501,13 +7540,13 @@
       </c>
       <c r="G34" s="111">
         <f t="shared" si="4"/>
-        <v>51710.373160112889</v>
+        <v>53132.408422016</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M34" s="79" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N34" s="80">
         <f>N31*N32*N33</f>
@@ -7547,7 +7586,7 @@
       </c>
       <c r="G35" s="111">
         <f t="shared" si="4"/>
-        <v>51859.877303952155</v>
+        <v>53286.023929810843</v>
       </c>
       <c r="M35" s="54"/>
       <c r="N35" s="55"/>
@@ -7585,7 +7624,7 @@
       </c>
       <c r="G36" s="111">
         <f t="shared" si="4"/>
-        <v>49955.139854335939</v>
+        <v>51328.906200330173</v>
       </c>
       <c r="M36" s="54"/>
       <c r="N36" s="73"/>
@@ -7623,7 +7662,7 @@
       </c>
       <c r="G37" s="111">
         <f t="shared" si="4"/>
-        <v>25049.335918703564</v>
+        <v>25738.192656467909</v>
       </c>
       <c r="P37" s="22">
         <v>1985</v>
@@ -7658,8 +7697,8 @@
         <f>D38</f>
         <v>0</v>
       </c>
-      <c r="M38" s="118" t="s">
-        <v>72</v>
+      <c r="M38" s="116" t="s">
+        <v>67</v>
       </c>
       <c r="P38" s="2">
         <v>1984</v>
@@ -7695,9 +7734,9 @@
         <v>0</v>
       </c>
       <c r="M39" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="N39" s="119">
+        <v>74</v>
+      </c>
+      <c r="N39" s="117">
         <v>8.33</v>
       </c>
       <c r="P39" s="2">
@@ -7734,11 +7773,11 @@
         <v>0</v>
       </c>
       <c r="M40" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="N40" s="120">
-        <f>G3</f>
-        <v>46219.848429433448</v>
+        <v>62</v>
+      </c>
+      <c r="N40" s="118">
+        <f>G3*0.15</f>
+        <v>7123.6341391864307</v>
       </c>
       <c r="P40" s="2">
         <v>1982</v>
@@ -7774,9 +7813,9 @@
         <v>0</v>
       </c>
       <c r="M41" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="N41" s="121">
+        <v>75</v>
+      </c>
+      <c r="N41" s="119">
         <f>1</f>
         <v>1</v>
       </c>
@@ -7814,9 +7853,9 @@
         <v>0</v>
       </c>
       <c r="M42" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="N42" s="121">
+        <v>76</v>
+      </c>
+      <c r="N42" s="119">
         <v>40</v>
       </c>
       <c r="P42" s="2">
@@ -7853,11 +7892,11 @@
         <v>0</v>
       </c>
       <c r="M43" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="N43" s="120">
-        <f>N40*(N39/100)*(N41/N42)</f>
-        <v>96.25283435429516</v>
+        <v>63</v>
+      </c>
+      <c r="N43" s="118">
+        <f>N40*(N39/100)/N42</f>
+        <v>14.834968094855743</v>
       </c>
       <c r="P43" s="2">
         <v>1979</v>
@@ -7893,11 +7932,11 @@
         <v>0</v>
       </c>
       <c r="M44" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="N44" s="121">
-        <f>J49</f>
-        <v>0</v>
+        <v>32</v>
+      </c>
+      <c r="N44" s="119">
+        <f>N14</f>
+        <v>33</v>
       </c>
       <c r="P44" s="2">
         <v>1978</v>
@@ -7933,11 +7972,11 @@
         <v>0</v>
       </c>
       <c r="M45" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="N45" s="123">
+        <v>64</v>
+      </c>
+      <c r="N45" s="121">
         <f>N43*(1-(N44/100))</f>
-        <v>96.25283435429516</v>
+        <v>9.9394286235533471</v>
       </c>
       <c r="P45" s="2">
         <v>1977</v>
@@ -8005,7 +8044,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M47" s="118"/>
+      <c r="M47" s="116"/>
       <c r="P47" s="2">
         <v>1975</v>
       </c>
@@ -8105,9 +8144,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M50" s="118" t="s">
-        <v>73</v>
-      </c>
+      <c r="M50" s="116"/>
       <c r="P50" s="2">
         <v>1972</v>
       </c>
@@ -8141,9 +8178,6 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M51" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="P51" s="2">
         <v>1971</v>
       </c>
@@ -8176,9 +8210,6 @@
       <c r="G52" s="111">
         <f t="shared" si="5"/>
         <v>0</v>
-      </c>
-      <c r="M52" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="P52" s="2">
         <v>1970</v>

</xml_diff>

<commit_message>
SRG est fucking masculin
</commit_message>
<xml_diff>
--- a/propre.xlsx
+++ b/propre.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\Université\Session-2-H-2020\ACT-1005-Analyse-et-traitement-collectif-du-risque\Calcul-Prestations\ATCR-TP2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\ATCR-TP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF92E762-DFD5-4C32-99A8-9FF87D770B16}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8773D1-A8AD-45C1-BC76-3C7E870514E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{47FD59A7-3964-46FC-BE03-C6B259F3D8B0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{47FD59A7-3964-46FC-BE03-C6B259F3D8B0}"/>
   </bookViews>
   <sheets>
     <sheet name="QUESTION 1" sheetId="1" r:id="rId1"/>
@@ -147,13 +147,7 @@
     <t xml:space="preserve">Indexation de la PSV </t>
   </si>
   <si>
-    <t xml:space="preserve">Indexation de la SRG célibataire </t>
-  </si>
-  <si>
     <t>*Les premiers 3500$ du revenu de Virginie ne sont</t>
-  </si>
-  <si>
-    <t>pas pris en compte pour la diminution de la SRG.</t>
   </si>
   <si>
     <t>Période cotisable (en années, 18 à 65 ans)</t>
@@ -285,7 +279,13 @@
     <t>revenus trop élevés.</t>
   </si>
   <si>
-    <t>Montant de la SRG après diminution selon les autres revenus</t>
+    <t xml:space="preserve">Indexation du SRG célibataire </t>
+  </si>
+  <si>
+    <t>Montant du SRG après diminution selon les autres revenus</t>
+  </si>
+  <si>
+    <t>pas pris en compte pour la diminution du SRG.</t>
   </si>
 </sst>
 </file>
@@ -1617,33 +1617,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D97A01-C9B7-4676-858F-079C6C4177D4}">
   <dimension ref="B1:R62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="96" workbookViewId="0">
+    <sheetView zoomScale="54" workbookViewId="0">
       <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="2"/>
-    <col min="3" max="3" width="11.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" style="5"/>
-    <col min="5" max="5" width="11.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="10.88671875" style="1"/>
-    <col min="11" max="11" width="47.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.88671875" style="1"/>
+    <col min="1" max="1" width="2.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="2"/>
+    <col min="3" max="3" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="5"/>
+    <col min="5" max="5" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="10.85546875" style="1"/>
+    <col min="11" max="11" width="47.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.85546875" style="1"/>
     <col min="14" max="14" width="48" style="1" customWidth="1"/>
-    <col min="15" max="16" width="10.88671875" style="1"/>
-    <col min="17" max="17" width="48.33203125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.88671875" style="1"/>
+    <col min="15" max="16" width="10.85546875" style="1"/>
+    <col min="17" max="17" width="48.28515625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="9.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:18" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="60" t="s">
         <v>0</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G2" s="36" t="s">
         <v>21</v>
@@ -1666,7 +1666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="61">
         <v>2019</v>
       </c>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="O3" s="126"/>
       <c r="Q3" s="116" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
@@ -1730,13 +1730,13 @@
         <v>57400</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="R4" s="117">
         <v>8.33</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B5" s="62">
         <v>2017</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>7217</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R5" s="118">
         <f>G3*0.15</f>
@@ -1806,7 +1806,7 @@
         <v>2.75E-2</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R6" s="119">
         <v>1</v>
@@ -1843,7 +1843,7 @@
         <v>10779.84</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="R7" s="119">
         <v>40</v>
@@ -1881,17 +1881,17 @@
         <v>42</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R8" s="118">
         <f>R5*(R4/100)/R7</f>
         <v>14.440796837832812</v>
       </c>
     </row>
-    <row r="9" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="62">
         <v>2013</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>0</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="O9" s="28">
         <f>AVERAGE(E3:E6,F3)</f>
@@ -1930,7 +1930,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="62">
         <v>2012</v>
       </c>
@@ -1963,14 +1963,14 @@
         <v>35</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R10" s="118">
         <f>R8*(1-(R9/100))</f>
         <v>9.6753338813479832</v>
       </c>
     </row>
-    <row r="11" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="62">
         <v>2011</v>
       </c>
@@ -2003,11 +2003,11 @@
         <v>5.25</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R11" s="117"/>
     </row>
-    <row r="12" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="62">
         <v>2010</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>47674.169658871557</v>
       </c>
       <c r="Q12" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R12" s="120"/>
     </row>
@@ -2085,7 +2085,7 @@
         <v>52006.787042566488</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N14" s="12" t="s">
         <v>32</v>
@@ -2095,7 +2095,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="62">
         <v>2007</v>
       </c>
@@ -2114,17 +2114,17 @@
         <v>52285.199316057529</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N15" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O15" s="29">
         <f>O13*(1-O14/100)</f>
         <v>7985.423417860985</v>
       </c>
     </row>
-    <row r="16" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="62">
         <v>2006</v>
       </c>
@@ -2143,14 +2143,14 @@
         <v>52498.311056353821</v>
       </c>
       <c r="N16" s="122" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="O16" s="123">
         <f>O15+R10</f>
         <v>7995.0987517423328</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B17" s="62">
         <v>2005</v>
       </c>
@@ -2171,7 +2171,7 @@
       <c r="N17" s="54"/>
       <c r="O17" s="68"/>
     </row>
-    <row r="18" spans="2:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:15" ht="14.45" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="62">
         <v>2004</v>
       </c>
@@ -2217,7 +2217,7 @@
       </c>
       <c r="O19" s="32"/>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B20" s="62">
         <v>2002</v>
       </c>
@@ -2240,7 +2240,7 @@
       </c>
       <c r="O20" s="33"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B21" s="62">
         <v>2001</v>
       </c>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="O23" s="42"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B24" s="63">
         <v>1998</v>
       </c>
@@ -2351,7 +2351,7 @@
       </c>
       <c r="O25" s="44"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B26" s="22">
         <v>1996</v>
       </c>
@@ -2372,7 +2372,7 @@
       <c r="N26" s="12"/>
       <c r="O26" s="28"/>
     </row>
-    <row r="27" spans="2:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="22">
         <v>1995</v>
       </c>
@@ -3073,36 +3073,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{367AD372-2F5B-444E-901D-D02956C9F1AC}">
   <dimension ref="B1:R62"/>
   <sheetViews>
-    <sheetView topLeftCell="I12" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView topLeftCell="J1" zoomScale="72" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="2"/>
-    <col min="3" max="3" width="11.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" style="5"/>
-    <col min="5" max="5" width="10.88671875" style="6"/>
-    <col min="6" max="6" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" style="1"/>
-    <col min="9" max="9" width="47.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.88671875" style="1"/>
-    <col min="12" max="12" width="10.88671875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.88671875" style="1"/>
-    <col min="14" max="14" width="51.21875" style="1" customWidth="1"/>
-    <col min="15" max="16" width="10.88671875" style="1"/>
-    <col min="17" max="17" width="43.6640625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.88671875" style="1"/>
+    <col min="1" max="1" width="2.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="2"/>
+    <col min="3" max="3" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="5"/>
+    <col min="5" max="5" width="10.85546875" style="6"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="1"/>
+    <col min="9" max="9" width="47.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" style="1"/>
+    <col min="12" max="12" width="10.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" style="1"/>
+    <col min="14" max="14" width="51.28515625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="10.85546875" style="1"/>
+    <col min="17" max="17" width="43.7109375" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="9.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:18" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="60" t="s">
         <v>0</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G2" s="36" t="s">
         <v>21</v>
@@ -3125,7 +3125,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="61">
         <v>2019</v>
       </c>
@@ -3155,7 +3155,7 @@
       </c>
       <c r="O3" s="126"/>
       <c r="Q3" s="116" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
@@ -3189,13 +3189,13 @@
         <v>57400</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="R4" s="117">
         <v>8.33</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B5" s="62">
         <v>2017</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>7217</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R5" s="118">
         <f>G3*0.15</f>
@@ -3266,7 +3266,7 @@
         <v>2.75E-2</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R6" s="119">
         <v>1</v>
@@ -3304,7 +3304,7 @@
         <v>10779.84</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="R7" s="119">
         <v>40</v>
@@ -3342,17 +3342,17 @@
         <v>42</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R8" s="118">
         <f>R5*(R4/100)/R7</f>
         <v>14.440796837832812</v>
       </c>
     </row>
-    <row r="9" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="62">
         <v>2013</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="62">
         <v>2012</v>
       </c>
@@ -3424,14 +3424,14 @@
         <v>35</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R10" s="118">
         <f>R8*(1-(R9/100))</f>
         <v>9.6753338813479832</v>
       </c>
     </row>
-    <row r="11" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="62">
         <v>2011</v>
       </c>
@@ -3464,11 +3464,11 @@
         <v>5.25</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R11" s="117"/>
     </row>
-    <row r="12" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="62">
         <v>2010</v>
       </c>
@@ -3494,11 +3494,11 @@
         <v>47674.169658871557</v>
       </c>
       <c r="Q12" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R12" s="120"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B13" s="62">
         <v>2009</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>11918.542414717889</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B14" s="62">
         <v>2008</v>
       </c>
@@ -3550,7 +3550,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="62">
         <v>2007</v>
       </c>
@@ -3569,14 +3569,14 @@
         <v>52285.199316057529</v>
       </c>
       <c r="N15" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O15" s="29">
         <f>O13*(1-O14/100)</f>
         <v>7985.423417860985</v>
       </c>
     </row>
-    <row r="16" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="62">
         <v>2006</v>
       </c>
@@ -3595,14 +3595,14 @@
         <v>52498.311056353821</v>
       </c>
       <c r="N16" s="124" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="O16" s="123">
         <f>O15+R10</f>
         <v>7995.0987517423328</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B17" s="62">
         <v>2005</v>
       </c>
@@ -3623,7 +3623,7 @@
       <c r="N17" s="54"/>
       <c r="O17" s="68"/>
     </row>
-    <row r="18" spans="2:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:15" ht="14.45" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="62">
         <v>2004</v>
       </c>
@@ -3669,7 +3669,7 @@
       </c>
       <c r="O19" s="32"/>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B20" s="62">
         <v>2002</v>
       </c>
@@ -3692,7 +3692,7 @@
       </c>
       <c r="O20" s="33"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B21" s="62">
         <v>2001</v>
       </c>
@@ -3759,7 +3759,7 @@
       </c>
       <c r="O23" s="42"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B24" s="63">
         <v>1998</v>
       </c>
@@ -3803,7 +3803,7 @@
       </c>
       <c r="O25" s="44"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B26" s="22">
         <v>1996</v>
       </c>
@@ -3824,7 +3824,7 @@
       <c r="N26" s="12"/>
       <c r="O26" s="28"/>
     </row>
-    <row r="27" spans="2:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="22">
         <v>1995</v>
       </c>
@@ -3847,7 +3847,7 @@
       </c>
       <c r="O27" s="57"/>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B28" s="22">
         <v>1994</v>
       </c>
@@ -3868,7 +3868,7 @@
       <c r="N28" s="54"/>
       <c r="O28" s="55"/>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B29" s="22">
         <v>1993</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:15" ht="14.45" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="22">
         <v>1992</v>
       </c>
@@ -3906,11 +3906,11 @@
         <v>0</v>
       </c>
       <c r="N30" s="126" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O30" s="127"/>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B31" s="22">
         <v>1991</v>
       </c>
@@ -3936,7 +3936,7 @@
         <v>9156.5734834015293</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B32" s="65">
         <v>1990</v>
       </c>
@@ -3981,14 +3981,14 @@
         <v>54560.949239195957</v>
       </c>
       <c r="N33" s="78" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="O33" s="76">
         <f>O7*(1+O6)^6</f>
         <v>12685.37464874215</v>
       </c>
     </row>
-    <row r="34" spans="2:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="66">
         <v>1988</v>
       </c>
@@ -4007,14 +4007,14 @@
         <v>51464.342565125393</v>
       </c>
       <c r="N34" s="79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O34" s="80">
         <f>O33-((O31-3500)/2)</f>
         <v>9857.0879070413866</v>
       </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B35" s="66">
         <v>1987</v>
       </c>
@@ -4033,11 +4033,11 @@
         <v>51612.344596031639</v>
       </c>
       <c r="N35" s="54" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O35" s="55"/>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B36" s="66">
         <v>1986</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>49717.203817896094</v>
       </c>
       <c r="N36" s="54" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="O36" s="73"/>
     </row>
@@ -4578,34 +4578,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF3058D-9527-44EF-BE25-5C09CA35E4DB}">
   <dimension ref="B1:R67"/>
   <sheetViews>
-    <sheetView topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView topLeftCell="I18" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="2"/>
-    <col min="3" max="3" width="11.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="2"/>
+    <col min="3" max="3" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="5" customWidth="1"/>
     <col min="5" max="5" width="11" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.88671875" style="1"/>
-    <col min="9" max="9" width="47.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.88671875" style="1"/>
-    <col min="13" max="13" width="49.5546875" style="1" customWidth="1"/>
-    <col min="14" max="16" width="10.88671875" style="1"/>
-    <col min="17" max="17" width="43.88671875" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.88671875" style="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="1"/>
+    <col min="9" max="9" width="47.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.85546875" style="1"/>
+    <col min="13" max="13" width="49.5703125" style="1" customWidth="1"/>
+    <col min="14" max="16" width="10.85546875" style="1"/>
+    <col min="17" max="17" width="43.85546875" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="9.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:18" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="60" t="s">
         <v>0</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G2" s="89" t="s">
         <v>21</v>
@@ -4628,7 +4628,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="61">
         <v>2024</v>
       </c>
@@ -4659,7 +4659,7 @@
       </c>
       <c r="N3" s="126"/>
       <c r="Q3" s="116" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
@@ -4694,13 +4694,13 @@
         <v>57400</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="R4" s="117">
         <v>8.33</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B5" s="62">
         <v>2022</v>
       </c>
@@ -4733,7 +4733,7 @@
         <v>7217</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R5" s="118">
         <f>G8*0.15+G7*0.3+G6*0.5+G5*0.75+G4+G3</f>
@@ -4773,7 +4773,7 @@
         <v>2.75E-2</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="R6" s="119">
         <f>B3-B8+1</f>
@@ -4813,7 +4813,7 @@
         <v>10779.84</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="R7" s="119">
         <v>40</v>
@@ -4843,24 +4843,24 @@
         <v>0</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N8" s="31">
         <f>65-18</f>
         <v>47</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R8" s="118">
         <f>R5*(R4/100)/R7</f>
         <v>407.95360556781873</v>
       </c>
     </row>
-    <row r="9" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="62">
         <v>2018</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="62">
         <v>2017</v>
       </c>
@@ -4932,14 +4932,14 @@
         <v>40</v>
       </c>
       <c r="Q10" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="R10" s="121">
         <f>R8*(1-(R9/100))</f>
         <v>407.95360556781873</v>
       </c>
     </row>
-    <row r="11" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="62">
         <v>2016</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B12" s="62">
         <v>2015</v>
       </c>
@@ -5018,7 +5018,7 @@
         <v>55968.130650666404</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M13" s="12" t="s">
         <v>30</v>
@@ -5028,7 +5028,7 @@
         <v>13990.611147342344</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B14" s="62">
         <v>2013</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="62">
         <v>2012</v>
       </c>
@@ -5072,17 +5072,17 @@
         <v>57039.616774356829</v>
       </c>
       <c r="M15" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N15" s="29">
         <f>N13*(1-N14/100)</f>
         <v>13990.611147342344</v>
       </c>
       <c r="Q15" s="116" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="62">
         <v>2011</v>
       </c>
@@ -5101,14 +5101,14 @@
         <v>57617.412422792535</v>
       </c>
       <c r="M16" s="122" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="N16" s="123">
         <f>N15+R10</f>
         <v>14398.564752910162</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
@@ -5132,10 +5132,10 @@
       <c r="M17" s="54"/>
       <c r="N17" s="68"/>
       <c r="Q17" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="2:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" ht="14.45" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="62">
         <v>2009</v>
       </c>
@@ -5181,7 +5181,7 @@
       </c>
       <c r="N19" s="32"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B20" s="62">
         <v>2007</v>
       </c>
@@ -5204,7 +5204,7 @@
       </c>
       <c r="N20" s="33"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B21" s="62">
         <v>2006</v>
       </c>
@@ -5271,7 +5271,7 @@
       </c>
       <c r="N23" s="42"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B24" s="62">
         <v>2003</v>
       </c>
@@ -5315,7 +5315,7 @@
       </c>
       <c r="N25" s="44"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B26" s="62">
         <v>2001</v>
       </c>
@@ -5336,7 +5336,7 @@
       <c r="M26" s="12"/>
       <c r="N26" s="28"/>
     </row>
-    <row r="27" spans="2:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="62">
         <v>2000</v>
       </c>
@@ -5359,7 +5359,7 @@
       </c>
       <c r="N27" s="57"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B28" s="62">
         <v>1999</v>
       </c>
@@ -5380,7 +5380,7 @@
       <c r="M28" s="54"/>
       <c r="N28" s="55"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B29" s="63">
         <v>1998</v>
       </c>
@@ -5399,7 +5399,7 @@
         <v>61432.518639727467</v>
       </c>
     </row>
-    <row r="30" spans="2:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:17" ht="14.45" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="22">
         <v>1997</v>
       </c>
@@ -5418,11 +5418,11 @@
         <v>0</v>
       </c>
       <c r="M30" s="126" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N30" s="127"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B31" s="22">
         <v>1996</v>
       </c>
@@ -5467,14 +5467,14 @@
         <v>2784.9782897580635</v>
       </c>
       <c r="M32" s="78" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="N32" s="76">
         <f>N7*(1+N6)^6</f>
         <v>12685.37464874215</v>
       </c>
     </row>
-    <row r="33" spans="2:14" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="22">
         <v>1994</v>
       </c>
@@ -5493,14 +5493,14 @@
         <v>0</v>
       </c>
       <c r="M33" s="79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N33" s="80">
         <f>N32-((N16-3500)/2)</f>
         <v>7236.0922722870691</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B34" s="22">
         <v>1993</v>
       </c>
@@ -5519,7 +5519,7 @@
         <v>0</v>
       </c>
       <c r="M34" s="54" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N34" s="55"/>
     </row>
@@ -5542,7 +5542,7 @@
         <v>0</v>
       </c>
       <c r="M35" s="54" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="N35" s="73"/>
     </row>
@@ -6164,32 +6164,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D06BBD0-3540-47FD-9C64-4AC625E42B0E}">
   <dimension ref="B1:T62"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="2"/>
-    <col min="3" max="3" width="11.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" style="5"/>
-    <col min="5" max="5" width="10.88671875" style="6"/>
-    <col min="6" max="6" width="12.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.88671875" style="1"/>
-    <col min="13" max="13" width="48.88671875" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.88671875" style="1"/>
+    <col min="1" max="1" width="2.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="2"/>
+    <col min="3" max="3" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="5"/>
+    <col min="5" max="5" width="10.85546875" style="6"/>
+    <col min="6" max="6" width="12.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.85546875" style="1"/>
+    <col min="13" max="13" width="48.85546875" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="9.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:20" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="2:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="60" t="s">
         <v>0</v>
       </c>
@@ -6203,13 +6203,13 @@
         <v>3</v>
       </c>
       <c r="F2" s="89" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G2" s="110" t="s">
         <v>21</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>4</v>
@@ -6218,7 +6218,7 @@
         <v>0</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>2</v>
@@ -6227,10 +6227,10 @@
         <v>3</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="2:20" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="101">
         <v>2019</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>57400</v>
       </c>
     </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:20" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B4" s="102">
         <v>2018</v>
       </c>
@@ -6318,7 +6318,7 @@
         <v>55863.746958637465</v>
       </c>
     </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:20" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B5" s="102">
         <v>2017</v>
       </c>
@@ -6487,7 +6487,7 @@
         <v>42</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P8" s="2">
         <v>2014</v>
@@ -6503,7 +6503,7 @@
         <v>50119.039527385365</v>
       </c>
     </row>
-    <row r="9" spans="2:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="102">
         <v>2013</v>
       </c>
@@ -6596,7 +6596,7 @@
         <v>47472.169383212604</v>
       </c>
     </row>
-    <row r="11" spans="2:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="102">
         <v>2011</v>
       </c>
@@ -6643,7 +6643,7 @@
         <v>46201.624703856542</v>
       </c>
     </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:20" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B12" s="102">
         <v>2010</v>
       </c>
@@ -6703,7 +6703,7 @@
         <v>52673.29061792195</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M13" s="12" t="s">
         <v>30</v>
@@ -6746,7 +6746,7 @@
         <v>53426.11933172663</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M14" s="12" t="s">
         <v>32</v>
@@ -6769,7 +6769,7 @@
         <v>42590.403675027614</v>
       </c>
     </row>
-    <row r="15" spans="2:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="102">
         <v>2007</v>
       </c>
@@ -6789,7 +6789,7 @@
         <v>53712.515857983111</v>
       </c>
       <c r="M15" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N15" s="29">
         <f>N13*(1-N14/100)</f>
@@ -6809,7 +6809,7 @@
         <v>41450.514525574319</v>
       </c>
     </row>
-    <row r="16" spans="2:20" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="102">
         <v>2006</v>
       </c>
@@ -6829,10 +6829,10 @@
         <v>53931.30079310407</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M16" s="122" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N16" s="123">
         <f>N15+N45</f>
@@ -6872,7 +6872,7 @@
         <v>54615.596525525048</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J17" s="115"/>
       <c r="M17" s="54"/>
@@ -6891,7 +6891,7 @@
         <v>39261.443657638127</v>
       </c>
     </row>
-    <row r="18" spans="2:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:19" ht="14.45" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="102">
         <v>2004</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>53673.993155453536</v>
       </c>
       <c r="M19" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N19" s="32"/>
       <c r="P19" s="2">
@@ -6986,7 +6986,7 @@
       </c>
       <c r="J20" s="35"/>
       <c r="M20" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N20" s="33"/>
       <c r="P20" s="2">
@@ -7003,7 +7003,7 @@
         <v>36192.682507625788</v>
       </c>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:19" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B21" s="102">
         <v>2001</v>
       </c>
@@ -7115,7 +7115,7 @@
         <v>33363.782506835174</v>
       </c>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:19" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B24" s="106">
         <v>1998</v>
       </c>
@@ -7193,7 +7193,7 @@
         <v>31601.785456477446</v>
       </c>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:19" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B26" s="106">
         <v>1996</v>
       </c>
@@ -7231,7 +7231,7 @@
         <v>30755.995578080237</v>
       </c>
     </row>
-    <row r="27" spans="2:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="106">
         <v>1995</v>
       </c>
@@ -7271,7 +7271,7 @@
         <v>29932.842411756919</v>
       </c>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:19" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B28" s="106">
         <v>1994</v>
       </c>
@@ -7307,7 +7307,7 @@
         <v>29131.720108765858</v>
       </c>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:19" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B29" s="106">
         <v>1993</v>
       </c>
@@ -7345,7 +7345,7 @@
         <v>28352.039035295238</v>
       </c>
     </row>
-    <row r="30" spans="2:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="106">
         <v>1992</v>
       </c>
@@ -7368,7 +7368,7 @@
         <v>54689.804116585801</v>
       </c>
       <c r="M30" s="126" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="N30" s="127"/>
       <c r="P30" s="22">
@@ -7385,7 +7385,7 @@
         <v>27593.225338486849</v>
       </c>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:19" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B31" s="106">
         <v>1991</v>
       </c>
@@ -7408,7 +7408,7 @@
         <v>55276.761955550952</v>
       </c>
       <c r="M31" s="77" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N31" s="75">
         <f>AVERAGE(D3:D7)</f>
@@ -7451,7 +7451,7 @@
         <v>54887.815210704131</v>
       </c>
       <c r="M32" s="78" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N32" s="92">
         <f>60-18</f>
@@ -7498,10 +7498,10 @@
         <v>25436.47790299587</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M33" s="78" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N33" s="93">
         <v>1.35E-2</v>
@@ -7520,7 +7520,7 @@
         <v>25436.47790299587</v>
       </c>
     </row>
-    <row r="34" spans="2:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:19" ht="14.45" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="106">
         <v>1988</v>
       </c>
@@ -7543,10 +7543,10 @@
         <v>53132.408422016</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M34" s="79" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="N34" s="80">
         <f>N31*N32*N33</f>
@@ -7566,7 +7566,7 @@
         <v>24755.696255957049</v>
       </c>
     </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:19" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B35" s="106">
         <v>1987</v>
       </c>
@@ -7604,7 +7604,7 @@
         <v>24093.135042293965</v>
       </c>
     </row>
-    <row r="36" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:19" ht="13.9" x14ac:dyDescent="0.25">
       <c r="B36" s="106">
         <v>1986</v>
       </c>
@@ -7678,7 +7678,7 @@
         <v>22820.736360588879</v>
       </c>
     </row>
-    <row r="38" spans="2:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="103">
         <v>1984</v>
       </c>
@@ -7698,7 +7698,7 @@
         <v>0</v>
       </c>
       <c r="M38" s="116" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P38" s="2">
         <v>1984</v>
@@ -7734,7 +7734,7 @@
         <v>0</v>
       </c>
       <c r="M39" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="N39" s="117">
         <v>8.33</v>
@@ -7773,7 +7773,7 @@
         <v>0</v>
       </c>
       <c r="M40" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N40" s="118">
         <f>G3*0.15</f>
@@ -7813,7 +7813,7 @@
         <v>0</v>
       </c>
       <c r="M41" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N41" s="119">
         <f>1</f>
@@ -7853,7 +7853,7 @@
         <v>0</v>
       </c>
       <c r="M42" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N42" s="119">
         <v>40</v>
@@ -7892,7 +7892,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N43" s="118">
         <f>N40*(N39/100)/N42</f>
@@ -7952,7 +7952,7 @@
         <v>18873.690974904424</v>
       </c>
     </row>
-    <row r="45" spans="2:19" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="2">
         <v>1977</v>
       </c>
@@ -7972,7 +7972,7 @@
         <v>0</v>
       </c>
       <c r="M45" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N45" s="121">
         <f>N43*(1-(N44/100))</f>

</xml_diff>

<commit_message>
modifier le nombre d'année dans le RCR
</commit_message>
<xml_diff>
--- a/propre.xlsx
+++ b/propre.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28615"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\ATCR-TP2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristanmetivier-dionne/ATCR-TP2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8773D1-A8AD-45C1-BC76-3C7E870514E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{47FD59A7-3964-46FC-BE03-C6B259F3D8B0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="QUESTION 1" sheetId="1" r:id="rId1"/>
@@ -18,9 +17,15 @@
     <sheet name="QUESTION 3" sheetId="3" r:id="rId3"/>
     <sheet name="QUESTION 6" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -291,7 +296,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
@@ -380,33 +385,33 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -415,7 +420,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -424,23 +429,23 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -448,101 +453,101 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -550,10 +555,10 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -561,42 +566,42 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -618,10 +623,10 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -629,7 +634,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -637,11 +642,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -672,7 +677,7 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -824,7 +829,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -884,23 +889,23 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -997,10 +1002,10 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1008,24 +1013,24 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1614,36 +1619,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D97A01-C9B7-4676-858F-079C6C4177D4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R62"/>
   <sheetViews>
-    <sheetView zoomScale="54" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView topLeftCell="J4" zoomScale="110" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="2"/>
-    <col min="3" max="3" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="5"/>
-    <col min="5" max="5" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="10.85546875" style="1"/>
-    <col min="11" max="11" width="47.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.85546875" style="1"/>
+    <col min="1" max="1" width="2.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="5"/>
+    <col min="5" max="5" width="11.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="47.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.83203125" style="1"/>
     <col min="14" max="14" width="48" style="1" customWidth="1"/>
-    <col min="15" max="16" width="10.85546875" style="1"/>
-    <col min="17" max="17" width="48.28515625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.85546875" style="1"/>
+    <col min="15" max="16" width="10.83203125" style="1"/>
+    <col min="17" max="17" width="48.33203125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:18" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B2" s="60" t="s">
         <v>0</v>
       </c>
@@ -1666,7 +1671,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" ht="16" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B3" s="61">
         <v>2019</v>
       </c>
@@ -1699,7 +1704,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B4" s="62">
         <v>2018</v>
       </c>
@@ -1736,7 +1741,7 @@
         <v>8.33</v>
       </c>
     </row>
-    <row r="5" spans="2:18" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B5" s="62">
         <v>2017</v>
       </c>
@@ -1775,7 +1780,7 @@
         <v>6934.3562246496103</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B6" s="62">
         <v>2016</v>
       </c>
@@ -1812,7 +1817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B7" s="62">
         <v>2015</v>
       </c>
@@ -1849,7 +1854,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B8" s="62">
         <v>2014</v>
       </c>
@@ -1891,7 +1896,7 @@
         <v>14.440796837832812</v>
       </c>
     </row>
-    <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B9" s="62">
         <v>2013</v>
       </c>
@@ -1930,7 +1935,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B10" s="62">
         <v>2012</v>
       </c>
@@ -1970,7 +1975,7 @@
         <v>9.6753338813479832</v>
       </c>
     </row>
-    <row r="11" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B11" s="62">
         <v>2011</v>
       </c>
@@ -2007,7 +2012,7 @@
       </c>
       <c r="R11" s="117"/>
     </row>
-    <row r="12" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B12" s="62">
         <v>2010</v>
       </c>
@@ -2037,7 +2042,7 @@
       </c>
       <c r="R12" s="120"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B13" s="62">
         <v>2009</v>
       </c>
@@ -2066,7 +2071,7 @@
         <v>11918.542414717889</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B14" s="62">
         <v>2008</v>
       </c>
@@ -2095,7 +2100,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B15" s="62">
         <v>2007</v>
       </c>
@@ -2124,7 +2129,7 @@
         <v>7985.423417860985</v>
       </c>
     </row>
-    <row r="16" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B16" s="62">
         <v>2006</v>
       </c>
@@ -2150,7 +2155,7 @@
         <v>7995.0987517423328</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B17" s="62">
         <v>2005</v>
       </c>
@@ -2171,7 +2176,7 @@
       <c r="N17" s="54"/>
       <c r="O17" s="68"/>
     </row>
-    <row r="18" spans="2:15" ht="14.45" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B18" s="62">
         <v>2004</v>
       </c>
@@ -2194,7 +2199,7 @@
       </c>
       <c r="O18" s="126"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B19" s="62">
         <v>2003</v>
       </c>
@@ -2217,7 +2222,7 @@
       </c>
       <c r="O19" s="32"/>
     </row>
-    <row r="20" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B20" s="62">
         <v>2002</v>
       </c>
@@ -2240,7 +2245,7 @@
       </c>
       <c r="O20" s="33"/>
     </row>
-    <row r="21" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B21" s="62">
         <v>2001</v>
       </c>
@@ -2261,7 +2266,7 @@
       <c r="N21" s="12"/>
       <c r="O21" s="28"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B22" s="62">
         <v>2000</v>
       </c>
@@ -2284,7 +2289,7 @@
       </c>
       <c r="O22" s="41"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B23" s="62">
         <v>1999</v>
       </c>
@@ -2307,7 +2312,7 @@
       </c>
       <c r="O23" s="42"/>
     </row>
-    <row r="24" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B24" s="63">
         <v>1998</v>
       </c>
@@ -2328,7 +2333,7 @@
       <c r="N24" s="12"/>
       <c r="O24" s="28"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B25" s="22">
         <v>1997</v>
       </c>
@@ -2351,7 +2356,7 @@
       </c>
       <c r="O25" s="44"/>
     </row>
-    <row r="26" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B26" s="22">
         <v>1996</v>
       </c>
@@ -2372,7 +2377,7 @@
       <c r="N26" s="12"/>
       <c r="O26" s="28"/>
     </row>
-    <row r="27" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B27" s="22">
         <v>1995</v>
       </c>
@@ -2395,7 +2400,7 @@
       </c>
       <c r="O27" s="57"/>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B28" s="22">
         <v>1994</v>
       </c>
@@ -2414,7 +2419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B29" s="22">
         <v>1993</v>
       </c>
@@ -2433,7 +2438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B30" s="22">
         <v>1992</v>
       </c>
@@ -2452,7 +2457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B31" s="22">
         <v>1991</v>
       </c>
@@ -2471,7 +2476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B32" s="65">
         <v>1990</v>
       </c>
@@ -2490,7 +2495,7 @@
         <v>53164.40134139463</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B33" s="66">
         <v>1989</v>
       </c>
@@ -2509,7 +2514,7 @@
         <v>54560.949239195957</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B34" s="66">
         <v>1988</v>
       </c>
@@ -2528,7 +2533,7 @@
         <v>51464.342565125393</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B35" s="66">
         <v>1987</v>
       </c>
@@ -2547,7 +2552,7 @@
         <v>51612.344596031639</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B36" s="66">
         <v>1986</v>
       </c>
@@ -2566,7 +2571,7 @@
         <v>49717.203817896094</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B37" s="66">
         <v>1985</v>
       </c>
@@ -2585,7 +2590,7 @@
         <v>48651.835164655473</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B38" s="66">
         <v>1984</v>
       </c>
@@ -2604,7 +2609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B39" s="67">
         <v>1983</v>
       </c>
@@ -2623,7 +2628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B40" s="21">
         <v>1982</v>
       </c>
@@ -2642,7 +2647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B41" s="21">
         <v>1981</v>
       </c>
@@ -2661,7 +2666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B42" s="21">
         <v>1980</v>
       </c>
@@ -2680,7 +2685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B43" s="21">
         <v>1979</v>
       </c>
@@ -2699,7 +2704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B44" s="21">
         <v>1978</v>
       </c>
@@ -2718,7 +2723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B45" s="2">
         <v>1977</v>
       </c>
@@ -2737,7 +2742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B46" s="2">
         <v>1976</v>
       </c>
@@ -2756,7 +2761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B47" s="2">
         <v>1975</v>
       </c>
@@ -2775,7 +2780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B48" s="2">
         <v>1974</v>
       </c>
@@ -2794,7 +2799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B49" s="2">
         <v>1973</v>
       </c>
@@ -2813,7 +2818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B50" s="2">
         <v>1972</v>
       </c>
@@ -2832,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B51" s="2">
         <v>1971</v>
       </c>
@@ -2851,7 +2856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B52" s="2">
         <v>1970</v>
       </c>
@@ -2870,7 +2875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B53" s="2">
         <v>1969</v>
       </c>
@@ -2889,7 +2894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B54" s="2">
         <v>1968</v>
       </c>
@@ -2908,7 +2913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B55" s="2">
         <v>1967</v>
       </c>
@@ -2927,7 +2932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B56" s="2">
         <v>1966</v>
       </c>
@@ -2946,7 +2951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B57" s="2">
         <v>1965</v>
       </c>
@@ -2965,7 +2970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B58" s="2">
         <v>1964</v>
       </c>
@@ -2984,7 +2989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B59" s="2">
         <v>1963</v>
       </c>
@@ -3003,7 +3008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B60" s="2">
         <v>1962</v>
       </c>
@@ -3022,7 +3027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B61" s="2">
         <v>1961</v>
       </c>
@@ -3041,7 +3046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B62" s="25">
         <v>1960</v>
       </c>
@@ -3070,39 +3075,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{367AD372-2F5B-444E-901D-D02956C9F1AC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R62"/>
   <sheetViews>
     <sheetView topLeftCell="J1" zoomScale="72" workbookViewId="0">
       <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="2"/>
-    <col min="3" max="3" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="5"/>
-    <col min="5" max="5" width="10.85546875" style="6"/>
-    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="1"/>
-    <col min="9" max="9" width="47.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" style="1"/>
-    <col min="12" max="12" width="10.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" style="1"/>
-    <col min="14" max="14" width="51.28515625" style="1" customWidth="1"/>
-    <col min="15" max="16" width="10.85546875" style="1"/>
-    <col min="17" max="17" width="43.7109375" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.85546875" style="1"/>
+    <col min="1" max="1" width="2.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="5"/>
+    <col min="5" max="5" width="10.83203125" style="6"/>
+    <col min="6" max="6" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="47.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="1"/>
+    <col min="12" max="12" width="10.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" style="1"/>
+    <col min="14" max="14" width="51.33203125" style="1" customWidth="1"/>
+    <col min="15" max="16" width="10.83203125" style="1"/>
+    <col min="17" max="17" width="43.6640625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:18" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B2" s="60" t="s">
         <v>0</v>
       </c>
@@ -3125,7 +3130,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" ht="16" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B3" s="61">
         <v>2019</v>
       </c>
@@ -3158,7 +3163,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B4" s="62">
         <v>2018</v>
       </c>
@@ -3195,7 +3200,7 @@
         <v>8.33</v>
       </c>
     </row>
-    <row r="5" spans="2:18" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B5" s="62">
         <v>2017</v>
       </c>
@@ -3234,7 +3239,7 @@
         <v>6934.3562246496103</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B6" s="62">
         <v>2016</v>
       </c>
@@ -3272,7 +3277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B7" s="62">
         <v>2015</v>
       </c>
@@ -3310,7 +3315,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B8" s="62">
         <v>2014</v>
       </c>
@@ -3352,7 +3357,7 @@
         <v>14.440796837832812</v>
       </c>
     </row>
-    <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B9" s="62">
         <v>2013</v>
       </c>
@@ -3391,7 +3396,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B10" s="62">
         <v>2012</v>
       </c>
@@ -3431,7 +3436,7 @@
         <v>9.6753338813479832</v>
       </c>
     </row>
-    <row r="11" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B11" s="62">
         <v>2011</v>
       </c>
@@ -3468,7 +3473,7 @@
       </c>
       <c r="R11" s="117"/>
     </row>
-    <row r="12" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B12" s="62">
         <v>2010</v>
       </c>
@@ -3498,7 +3503,7 @@
       </c>
       <c r="R12" s="120"/>
     </row>
-    <row r="13" spans="2:18" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B13" s="62">
         <v>2009</v>
       </c>
@@ -3524,7 +3529,7 @@
         <v>11918.542414717889</v>
       </c>
     </row>
-    <row r="14" spans="2:18" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B14" s="62">
         <v>2008</v>
       </c>
@@ -3550,7 +3555,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B15" s="62">
         <v>2007</v>
       </c>
@@ -3576,7 +3581,7 @@
         <v>7985.423417860985</v>
       </c>
     </row>
-    <row r="16" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B16" s="62">
         <v>2006</v>
       </c>
@@ -3602,7 +3607,7 @@
         <v>7995.0987517423328</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B17" s="62">
         <v>2005</v>
       </c>
@@ -3623,7 +3628,7 @@
       <c r="N17" s="54"/>
       <c r="O17" s="68"/>
     </row>
-    <row r="18" spans="2:15" ht="14.45" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B18" s="62">
         <v>2004</v>
       </c>
@@ -3646,7 +3651,7 @@
       </c>
       <c r="O18" s="126"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B19" s="62">
         <v>2003</v>
       </c>
@@ -3669,7 +3674,7 @@
       </c>
       <c r="O19" s="32"/>
     </row>
-    <row r="20" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B20" s="62">
         <v>2002</v>
       </c>
@@ -3692,7 +3697,7 @@
       </c>
       <c r="O20" s="33"/>
     </row>
-    <row r="21" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B21" s="62">
         <v>2001</v>
       </c>
@@ -3713,7 +3718,7 @@
       <c r="N21" s="12"/>
       <c r="O21" s="28"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B22" s="62">
         <v>2000</v>
       </c>
@@ -3736,7 +3741,7 @@
       </c>
       <c r="O22" s="41"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B23" s="62">
         <v>1999</v>
       </c>
@@ -3759,7 +3764,7 @@
       </c>
       <c r="O23" s="42"/>
     </row>
-    <row r="24" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B24" s="63">
         <v>1998</v>
       </c>
@@ -3780,7 +3785,7 @@
       <c r="N24" s="12"/>
       <c r="O24" s="28"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B25" s="22">
         <v>1997</v>
       </c>
@@ -3803,7 +3808,7 @@
       </c>
       <c r="O25" s="44"/>
     </row>
-    <row r="26" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B26" s="22">
         <v>1996</v>
       </c>
@@ -3824,7 +3829,7 @@
       <c r="N26" s="12"/>
       <c r="O26" s="28"/>
     </row>
-    <row r="27" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B27" s="22">
         <v>1995</v>
       </c>
@@ -3847,7 +3852,7 @@
       </c>
       <c r="O27" s="57"/>
     </row>
-    <row r="28" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B28" s="22">
         <v>1994</v>
       </c>
@@ -3868,7 +3873,7 @@
       <c r="N28" s="54"/>
       <c r="O28" s="55"/>
     </row>
-    <row r="29" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B29" s="22">
         <v>1993</v>
       </c>
@@ -3887,7 +3892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:15" ht="14.45" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B30" s="22">
         <v>1992</v>
       </c>
@@ -3910,7 +3915,7 @@
       </c>
       <c r="O30" s="127"/>
     </row>
-    <row r="31" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B31" s="22">
         <v>1991</v>
       </c>
@@ -3936,7 +3941,7 @@
         <v>9156.5734834015293</v>
       </c>
     </row>
-    <row r="32" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B32" s="65">
         <v>1990</v>
       </c>
@@ -3962,7 +3967,7 @@
         <v>8492.7372614038886</v>
       </c>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B33" s="66">
         <v>1989</v>
       </c>
@@ -3988,7 +3993,7 @@
         <v>12685.37464874215</v>
       </c>
     </row>
-    <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B34" s="66">
         <v>1988</v>
       </c>
@@ -4014,7 +4019,7 @@
         <v>9857.0879070413866</v>
       </c>
     </row>
-    <row r="35" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B35" s="66">
         <v>1987</v>
       </c>
@@ -4037,7 +4042,7 @@
       </c>
       <c r="O35" s="55"/>
     </row>
-    <row r="36" spans="2:15" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B36" s="66">
         <v>1986</v>
       </c>
@@ -4060,7 +4065,7 @@
       </c>
       <c r="O36" s="73"/>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B37" s="66">
         <v>1985</v>
       </c>
@@ -4081,7 +4086,7 @@
       <c r="N37" s="54"/>
       <c r="O37" s="72"/>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B38" s="66">
         <v>1984</v>
       </c>
@@ -4102,7 +4107,7 @@
       <c r="N38" s="54"/>
       <c r="O38" s="74"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B39" s="67">
         <v>1983</v>
       </c>
@@ -4123,7 +4128,7 @@
       <c r="N39" s="54"/>
       <c r="O39" s="74"/>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B40" s="21">
         <v>1982</v>
       </c>
@@ -4144,7 +4149,7 @@
       <c r="N40" s="54"/>
       <c r="O40" s="73"/>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B41" s="21">
         <v>1981</v>
       </c>
@@ -4165,7 +4170,7 @@
       <c r="N41" s="54"/>
       <c r="O41" s="55"/>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B42" s="21">
         <v>1980</v>
       </c>
@@ -4184,7 +4189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B43" s="21">
         <v>1979</v>
       </c>
@@ -4203,7 +4208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B44" s="21">
         <v>1978</v>
       </c>
@@ -4222,7 +4227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B45" s="2">
         <v>1977</v>
       </c>
@@ -4241,7 +4246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B46" s="2">
         <v>1976</v>
       </c>
@@ -4260,7 +4265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B47" s="2">
         <v>1975</v>
       </c>
@@ -4279,7 +4284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B48" s="2">
         <v>1974</v>
       </c>
@@ -4298,7 +4303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B49" s="2">
         <v>1973</v>
       </c>
@@ -4317,7 +4322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B50" s="2">
         <v>1972</v>
       </c>
@@ -4336,7 +4341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B51" s="2">
         <v>1971</v>
       </c>
@@ -4355,7 +4360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B52" s="2">
         <v>1970</v>
       </c>
@@ -4374,7 +4379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B53" s="2">
         <v>1969</v>
       </c>
@@ -4393,7 +4398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B54" s="2">
         <v>1968</v>
       </c>
@@ -4412,7 +4417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B55" s="2">
         <v>1967</v>
       </c>
@@ -4431,7 +4436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B56" s="2">
         <v>1966</v>
       </c>
@@ -4450,7 +4455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B57" s="2">
         <v>1965</v>
       </c>
@@ -4469,7 +4474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B58" s="2">
         <v>1964</v>
       </c>
@@ -4488,7 +4493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B59" s="2">
         <v>1963</v>
       </c>
@@ -4507,7 +4512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B60" s="2">
         <v>1962</v>
       </c>
@@ -4526,7 +4531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B61" s="2">
         <v>1961</v>
       </c>
@@ -4545,7 +4550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B62" s="25">
         <v>1960</v>
       </c>
@@ -4575,37 +4580,37 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF3058D-9527-44EF-BE25-5C09CA35E4DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R67"/>
   <sheetViews>
-    <sheetView topLeftCell="I18" workbookViewId="0">
+    <sheetView topLeftCell="H2" workbookViewId="0">
       <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="2"/>
-    <col min="3" max="3" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="11.5" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="5" customWidth="1"/>
     <col min="5" max="5" width="11" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="1"/>
-    <col min="9" max="9" width="47.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.85546875" style="1"/>
-    <col min="13" max="13" width="49.5703125" style="1" customWidth="1"/>
-    <col min="14" max="16" width="10.85546875" style="1"/>
-    <col min="17" max="17" width="43.85546875" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.85546875" style="1"/>
+    <col min="6" max="6" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="47.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="49.5" style="1" customWidth="1"/>
+    <col min="14" max="16" width="10.83203125" style="1"/>
+    <col min="17" max="17" width="43.83203125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:18" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B2" s="60" t="s">
         <v>0</v>
       </c>
@@ -4628,7 +4633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" ht="16" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B3" s="61">
         <v>2024</v>
       </c>
@@ -4662,7 +4667,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B4" s="62">
         <v>2023</v>
       </c>
@@ -4700,7 +4705,7 @@
         <v>8.33</v>
       </c>
     </row>
-    <row r="5" spans="2:18" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B5" s="62">
         <v>2022</v>
       </c>
@@ -4740,7 +4745,7 @@
         <v>195896.08910819629</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B6" s="62">
         <v>2021</v>
       </c>
@@ -4780,7 +4785,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B7" s="62">
         <v>2020</v>
       </c>
@@ -4819,7 +4824,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B8" s="62">
         <v>2019</v>
       </c>
@@ -4860,7 +4865,7 @@
         <v>407.95360556781873</v>
       </c>
     </row>
-    <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B9" s="62">
         <v>2018</v>
       </c>
@@ -4899,7 +4904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B10" s="62">
         <v>2017</v>
       </c>
@@ -4939,7 +4944,7 @@
         <v>407.95360556781873</v>
       </c>
     </row>
-    <row r="11" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B11" s="62">
         <v>2016</v>
       </c>
@@ -4972,7 +4977,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:18" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B12" s="62">
         <v>2015</v>
       </c>
@@ -4999,7 +5004,7 @@
       </c>
       <c r="Q12" s="116"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B13" s="62">
         <v>2014</v>
       </c>
@@ -5028,7 +5033,7 @@
         <v>13990.611147342344</v>
       </c>
     </row>
-    <row r="14" spans="2:18" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B14" s="62">
         <v>2013</v>
       </c>
@@ -5053,7 +5058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B15" s="62">
         <v>2012</v>
       </c>
@@ -5082,7 +5087,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B16" s="62">
         <v>2011</v>
       </c>
@@ -5111,7 +5116,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.15">
       <c r="B17" s="62">
         <v>2010</v>
       </c>
@@ -5135,7 +5140,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="2:17" ht="14.45" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B18" s="62">
         <v>2009</v>
       </c>
@@ -5158,7 +5163,7 @@
       </c>
       <c r="N18" s="126"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.15">
       <c r="B19" s="62">
         <v>2008</v>
       </c>
@@ -5181,7 +5186,7 @@
       </c>
       <c r="N19" s="32"/>
     </row>
-    <row r="20" spans="2:17" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.15">
       <c r="B20" s="62">
         <v>2007</v>
       </c>
@@ -5204,7 +5209,7 @@
       </c>
       <c r="N20" s="33"/>
     </row>
-    <row r="21" spans="2:17" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.15">
       <c r="B21" s="62">
         <v>2006</v>
       </c>
@@ -5225,7 +5230,7 @@
       <c r="M21" s="12"/>
       <c r="N21" s="28"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.15">
       <c r="B22" s="62">
         <v>2005</v>
       </c>
@@ -5248,7 +5253,7 @@
       </c>
       <c r="N22" s="41"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.15">
       <c r="B23" s="62">
         <v>2004</v>
       </c>
@@ -5271,7 +5276,7 @@
       </c>
       <c r="N23" s="42"/>
     </row>
-    <row r="24" spans="2:17" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.15">
       <c r="B24" s="62">
         <v>2003</v>
       </c>
@@ -5292,7 +5297,7 @@
       <c r="M24" s="12"/>
       <c r="N24" s="28"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.15">
       <c r="B25" s="62">
         <v>2002</v>
       </c>
@@ -5315,7 +5320,7 @@
       </c>
       <c r="N25" s="44"/>
     </row>
-    <row r="26" spans="2:17" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.15">
       <c r="B26" s="62">
         <v>2001</v>
       </c>
@@ -5336,7 +5341,7 @@
       <c r="M26" s="12"/>
       <c r="N26" s="28"/>
     </row>
-    <row r="27" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B27" s="62">
         <v>2000</v>
       </c>
@@ -5359,7 +5364,7 @@
       </c>
       <c r="N27" s="57"/>
     </row>
-    <row r="28" spans="2:17" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.15">
       <c r="B28" s="62">
         <v>1999</v>
       </c>
@@ -5380,7 +5385,7 @@
       <c r="M28" s="54"/>
       <c r="N28" s="55"/>
     </row>
-    <row r="29" spans="2:17" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.15">
       <c r="B29" s="63">
         <v>1998</v>
       </c>
@@ -5399,7 +5404,7 @@
         <v>61432.518639727467</v>
       </c>
     </row>
-    <row r="30" spans="2:17" ht="14.45" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B30" s="22">
         <v>1997</v>
       </c>
@@ -5422,7 +5427,7 @@
       </c>
       <c r="N30" s="127"/>
     </row>
-    <row r="31" spans="2:17" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.15">
       <c r="B31" s="22">
         <v>1996</v>
       </c>
@@ -5448,7 +5453,7 @@
         <v>8492.7372614038886</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.15">
       <c r="B32" s="22">
         <v>1995</v>
       </c>
@@ -5474,7 +5479,7 @@
         <v>12685.37464874215</v>
       </c>
     </row>
-    <row r="33" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B33" s="22">
         <v>1994</v>
       </c>
@@ -5500,7 +5505,7 @@
         <v>7236.0922722870691</v>
       </c>
     </row>
-    <row r="34" spans="2:14" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B34" s="22">
         <v>1993</v>
       </c>
@@ -5523,7 +5528,7 @@
       </c>
       <c r="N34" s="55"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B35" s="22">
         <v>1992</v>
       </c>
@@ -5546,7 +5551,7 @@
       </c>
       <c r="N35" s="73"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B36" s="22">
         <v>1991</v>
       </c>
@@ -5565,7 +5570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B37" s="61">
         <v>1990</v>
       </c>
@@ -5584,7 +5589,7 @@
         <v>60887.771708566332</v>
       </c>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B38" s="62">
         <v>1989</v>
       </c>
@@ -5603,7 +5608,7 @@
         <v>62487.200789604387</v>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B39" s="62">
         <v>1988</v>
       </c>
@@ -5622,7 +5627,7 @@
         <v>58940.739708790381</v>
       </c>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B40" s="62">
         <v>1987</v>
       </c>
@@ -5641,7 +5646,7 @@
         <v>59110.242489652272</v>
       </c>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B41" s="62">
         <v>1986</v>
       </c>
@@ -5660,7 +5665,7 @@
         <v>56939.788273235361</v>
       </c>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B42" s="62">
         <v>1985</v>
       </c>
@@ -5679,7 +5684,7 @@
         <v>55719.649953094602</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B43" s="67">
         <v>1984</v>
       </c>
@@ -5698,7 +5703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B44" s="21">
         <v>1983</v>
       </c>
@@ -5717,7 +5722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B45" s="21">
         <v>1982</v>
       </c>
@@ -5736,7 +5741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B46" s="21">
         <v>1981</v>
       </c>
@@ -5755,7 +5760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B47" s="21">
         <v>1980</v>
       </c>
@@ -5774,7 +5779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B48" s="21">
         <v>1979</v>
       </c>
@@ -5793,7 +5798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B49" s="21">
         <v>1978</v>
       </c>
@@ -5812,7 +5817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B50" s="2">
         <v>1977</v>
       </c>
@@ -5831,7 +5836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B51" s="2">
         <v>1976</v>
       </c>
@@ -5850,7 +5855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B52" s="2">
         <v>1975</v>
       </c>
@@ -5869,7 +5874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B53" s="2">
         <v>1974</v>
       </c>
@@ -5888,7 +5893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B54" s="2">
         <v>1973</v>
       </c>
@@ -5907,7 +5912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B55" s="2">
         <v>1972</v>
       </c>
@@ -5926,7 +5931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B56" s="2">
         <v>1971</v>
       </c>
@@ -5945,7 +5950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B57" s="2">
         <v>1970</v>
       </c>
@@ -5964,7 +5969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B58" s="2">
         <v>1969</v>
       </c>
@@ -5983,7 +5988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B59" s="2">
         <v>1968</v>
       </c>
@@ -6002,7 +6007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B60" s="2">
         <v>1967</v>
       </c>
@@ -6021,7 +6026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B61" s="2">
         <v>1966</v>
       </c>
@@ -6040,7 +6045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B62" s="2">
         <v>1965</v>
       </c>
@@ -6059,7 +6064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B63" s="2">
         <v>1964</v>
       </c>
@@ -6078,7 +6083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B64" s="2">
         <v>1963</v>
       </c>
@@ -6097,7 +6102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B65" s="2">
         <v>1962</v>
       </c>
@@ -6116,7 +6121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B66" s="2">
         <v>1961</v>
       </c>
@@ -6135,7 +6140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B67" s="25">
         <v>1960</v>
       </c>
@@ -6161,35 +6166,35 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D06BBD0-3540-47FD-9C64-4AC625E42B0E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="125" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="2"/>
-    <col min="3" max="3" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="5"/>
-    <col min="5" max="5" width="10.85546875" style="6"/>
-    <col min="6" max="6" width="12.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.85546875" style="1"/>
-    <col min="13" max="13" width="48.85546875" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.85546875" style="1"/>
+    <col min="1" max="1" width="2.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="5"/>
+    <col min="5" max="5" width="10.83203125" style="6"/>
+    <col min="6" max="6" width="12.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="48.83203125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:20" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B1" s="3"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B2" s="60" t="s">
         <v>0</v>
       </c>
@@ -6230,7 +6235,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:20" ht="16" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B3" s="101">
         <v>2019</v>
       </c>
@@ -6272,7 +6277,7 @@
         <v>57400</v>
       </c>
     </row>
-    <row r="4" spans="2:20" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B4" s="102">
         <v>2018</v>
       </c>
@@ -6296,7 +6301,7 @@
       </c>
       <c r="J4" s="27">
         <f>N34</f>
-        <v>26871.263999999999</v>
+        <v>22392.720000000001</v>
       </c>
       <c r="M4" s="11" t="s">
         <v>14</v>
@@ -6318,7 +6323,7 @@
         <v>55863.746958637465</v>
       </c>
     </row>
-    <row r="5" spans="2:20" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B5" s="102">
         <v>2017</v>
       </c>
@@ -6364,7 +6369,7 @@
         <v>54368.610178722593</v>
       </c>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B6" s="102">
         <v>2016</v>
       </c>
@@ -6409,7 +6414,7 @@
         <v>52913.489225034151</v>
       </c>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B7" s="102">
         <v>2015</v>
       </c>
@@ -6454,7 +6459,7 @@
         <v>51497.313114388468</v>
       </c>
     </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B8" s="102">
         <v>2014</v>
       </c>
@@ -6503,7 +6508,7 @@
         <v>50119.039527385365</v>
       </c>
     </row>
-    <row r="9" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B9" s="102">
         <v>2013</v>
       </c>
@@ -6549,7 +6554,7 @@
         <v>48777.654041250957</v>
       </c>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B10" s="102">
         <v>2012</v>
       </c>
@@ -6573,7 +6578,7 @@
       </c>
       <c r="J10" s="70">
         <f>SUM(J4:J5)</f>
-        <v>35403.609452032804</v>
+        <v>30925.065452032806</v>
       </c>
       <c r="M10" s="12" t="s">
         <v>23</v>
@@ -6596,7 +6601,7 @@
         <v>47472.169383212604</v>
       </c>
     </row>
-    <row r="11" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B11" s="102">
         <v>2011</v>
       </c>
@@ -6620,7 +6625,7 @@
       </c>
       <c r="J11" s="17">
         <f>J10/D3</f>
-        <v>0.72606405635718718</v>
+        <v>0.63421721154268385</v>
       </c>
       <c r="M11" s="12" t="s">
         <v>24</v>
@@ -6643,7 +6648,7 @@
         <v>46201.624703856542</v>
       </c>
     </row>
-    <row r="12" spans="2:20" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B12" s="102">
         <v>2010</v>
       </c>
@@ -6683,7 +6688,7 @@
         <v>44965.084869933373</v>
       </c>
     </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B13" s="102">
         <v>2009</v>
       </c>
@@ -6726,7 +6731,7 @@
         <v>43761.639776090873</v>
       </c>
     </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B14" s="102">
         <v>2008</v>
       </c>
@@ -6769,7 +6774,7 @@
         <v>42590.403675027614</v>
       </c>
     </row>
-    <row r="15" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B15" s="102">
         <v>2007</v>
       </c>
@@ -6809,7 +6814,7 @@
         <v>41450.514525574319</v>
       </c>
     </row>
-    <row r="16" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B16" s="102">
         <v>2006</v>
       </c>
@@ -6852,7 +6857,7 @@
         <v>40341.133358223182</v>
       </c>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B17" s="102">
         <v>2005</v>
       </c>
@@ -6891,7 +6896,7 @@
         <v>39261.443657638127</v>
       </c>
     </row>
-    <row r="18" spans="2:19" ht="14.45" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B18" s="102">
         <v>2004</v>
       </c>
@@ -6928,7 +6933,7 @@
         <v>38210.650761691606</v>
       </c>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B19" s="102">
         <v>2003</v>
       </c>
@@ -6965,7 +6970,7 @@
         <v>37187.981276585502</v>
       </c>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B20" s="102">
         <v>2002</v>
       </c>
@@ -7003,7 +7008,7 @@
         <v>36192.682507625788</v>
       </c>
     </row>
-    <row r="21" spans="2:19" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B21" s="102">
         <v>2001</v>
       </c>
@@ -7038,7 +7043,7 @@
         <v>35224.021905231908</v>
       </c>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B22" s="102">
         <v>2000</v>
       </c>
@@ -7075,7 +7080,7 @@
         <v>34281.286525773146</v>
       </c>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B23" s="106">
         <v>1999</v>
       </c>
@@ -7115,7 +7120,7 @@
         <v>33363.782506835174</v>
       </c>
     </row>
-    <row r="24" spans="2:19" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B24" s="106">
         <v>1998</v>
       </c>
@@ -7153,7 +7158,7 @@
         <v>32470.834556530579</v>
       </c>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B25" s="106">
         <v>1997</v>
       </c>
@@ -7193,7 +7198,7 @@
         <v>31601.785456477446</v>
       </c>
     </row>
-    <row r="26" spans="2:19" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B26" s="106">
         <v>1996</v>
       </c>
@@ -7231,7 +7236,7 @@
         <v>30755.995578080237</v>
       </c>
     </row>
-    <row r="27" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B27" s="106">
         <v>1995</v>
       </c>
@@ -7271,7 +7276,7 @@
         <v>29932.842411756919</v>
       </c>
     </row>
-    <row r="28" spans="2:19" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B28" s="106">
         <v>1994</v>
       </c>
@@ -7307,7 +7312,7 @@
         <v>29131.720108765858</v>
       </c>
     </row>
-    <row r="29" spans="2:19" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B29" s="106">
         <v>1993</v>
       </c>
@@ -7345,7 +7350,7 @@
         <v>28352.039035295238</v>
       </c>
     </row>
-    <row r="30" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B30" s="106">
         <v>1992</v>
       </c>
@@ -7385,7 +7390,7 @@
         <v>27593.225338486849</v>
       </c>
     </row>
-    <row r="31" spans="2:19" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B31" s="106">
         <v>1991</v>
       </c>
@@ -7428,7 +7433,7 @@
         <v>26854.72052407479</v>
       </c>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B32" s="106">
         <v>1990</v>
       </c>
@@ -7454,8 +7459,8 @@
         <v>44</v>
       </c>
       <c r="N32" s="92">
-        <f>60-18</f>
-        <v>42</v>
+        <f>60-25</f>
+        <v>35</v>
       </c>
       <c r="P32" s="22">
         <v>1990</v>
@@ -7471,7 +7476,7 @@
         <v>26135.981045328259</v>
       </c>
     </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B33" s="106">
         <v>1989</v>
       </c>
@@ -7520,7 +7525,7 @@
         <v>25436.47790299587</v>
       </c>
     </row>
-    <row r="34" spans="2:19" ht="14.45" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B34" s="106">
         <v>1988</v>
       </c>
@@ -7550,7 +7555,7 @@
       </c>
       <c r="N34" s="80">
         <f>N31*N32*N33</f>
-        <v>26871.263999999999</v>
+        <v>22392.720000000001</v>
       </c>
       <c r="P34" s="22">
         <v>1988</v>
@@ -7566,7 +7571,7 @@
         <v>24755.696255957049</v>
       </c>
     </row>
-    <row r="35" spans="2:19" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B35" s="106">
         <v>1987</v>
       </c>
@@ -7604,7 +7609,7 @@
         <v>24093.135042293965</v>
       </c>
     </row>
-    <row r="36" spans="2:19" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B36" s="106">
         <v>1986</v>
       </c>
@@ -7642,7 +7647,7 @@
         <v>23448.306610505075</v>
       </c>
     </row>
-    <row r="37" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B37" s="106">
         <v>1985</v>
       </c>
@@ -7678,7 +7683,7 @@
         <v>22820.736360588879</v>
       </c>
     </row>
-    <row r="38" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B38" s="103">
         <v>1984</v>
       </c>
@@ -7714,7 +7719,7 @@
         <v>22209.962394733699</v>
       </c>
     </row>
-    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B39" s="104">
         <v>1983</v>
       </c>
@@ -7753,7 +7758,7 @@
         <v>21615.535177356396</v>
       </c>
     </row>
-    <row r="40" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B40" s="104">
         <v>1982</v>
       </c>
@@ -7793,7 +7798,7 @@
         <v>21037.017204239801</v>
       </c>
     </row>
-    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B41" s="104">
         <v>1981</v>
       </c>
@@ -7833,7 +7838,7 @@
         <v>20473.982680525351</v>
       </c>
     </row>
-    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B42" s="104">
         <v>1980</v>
       </c>
@@ -7872,7 +7877,7 @@
         <v>19926.017207323941</v>
       </c>
     </row>
-    <row r="43" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B43" s="104">
         <v>1979</v>
       </c>
@@ -7912,7 +7917,7 @@
         <v>19392.717476714297</v>
       </c>
     </row>
-    <row r="44" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B44" s="105">
         <v>1978</v>
       </c>
@@ -7952,7 +7957,7 @@
         <v>18873.690974904424</v>
       </c>
     </row>
-    <row r="45" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B45" s="2">
         <v>1977</v>
       </c>
@@ -7992,7 +7997,7 @@
         <v>18368.555693337639</v>
       </c>
     </row>
-    <row r="46" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B46" s="2">
         <v>1976</v>
       </c>
@@ -8025,7 +8030,7 @@
         <v>17876.939847530546</v>
       </c>
     </row>
-    <row r="47" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B47" s="2">
         <v>1975</v>
       </c>
@@ -8059,7 +8064,7 @@
         <v>17398.481603436052</v>
       </c>
     </row>
-    <row r="48" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B48" s="2">
         <v>1974</v>
       </c>
@@ -8092,7 +8097,7 @@
         <v>16932.828811129977</v>
       </c>
     </row>
-    <row r="49" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B49" s="2">
         <v>1973</v>
       </c>
@@ -8125,7 +8130,7 @@
         <v>16479.638745625281</v>
       </c>
     </row>
-    <row r="50" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B50" s="2">
         <v>1972</v>
       </c>
@@ -8159,7 +8164,7 @@
         <v>16038.577854623143</v>
       </c>
     </row>
-    <row r="51" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B51" s="2">
         <v>1971</v>
       </c>
@@ -8192,7 +8197,7 @@
         <v>15609.321513015224</v>
       </c>
     </row>
-    <row r="52" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B52" s="2">
         <v>1970</v>
       </c>
@@ -8225,7 +8230,7 @@
         <v>15191.55378395642</v>
       </c>
     </row>
-    <row r="53" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B53" s="2">
         <v>1969</v>
       </c>
@@ -8258,7 +8263,7 @@
         <v>14784.967186332282</v>
       </c>
     </row>
-    <row r="54" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B54" s="2">
         <v>1968</v>
       </c>
@@ -8291,7 +8296,7 @@
         <v>14389.262468449908</v>
       </c>
     </row>
-    <row r="55" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B55" s="2">
         <v>1967</v>
       </c>
@@ -8324,7 +8329,7 @@
         <v>14004.148387785797</v>
       </c>
     </row>
-    <row r="56" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B56" s="2">
         <v>1966</v>
       </c>
@@ -8357,7 +8362,7 @@
         <v>13629.341496628513</v>
       </c>
     </row>
-    <row r="57" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B57" s="2">
         <v>1965</v>
       </c>
@@ -8390,7 +8395,7 @@
         <v>13264.565933458405</v>
       </c>
     </row>
-    <row r="58" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B58" s="2">
         <v>1964</v>
       </c>
@@ -8423,7 +8428,7 @@
         <v>12909.553219910855</v>
       </c>
     </row>
-    <row r="59" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B59" s="2">
         <v>1963</v>
       </c>
@@ -8456,7 +8461,7 @@
         <v>12564.04206317358</v>
       </c>
     </row>
-    <row r="60" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B60" s="2">
         <v>1962</v>
       </c>
@@ -8489,7 +8494,7 @@
         <v>12227.778163672583</v>
       </c>
     </row>
-    <row r="61" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B61" s="2">
         <v>1961</v>
       </c>
@@ -8522,7 +8527,7 @@
         <v>11900.51402790519</v>
       </c>
     </row>
-    <row r="62" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B62" s="2">
         <v>1960</v>
       </c>

</xml_diff>